<commit_message>
update steps by steps apply translation system
</commit_message>
<xml_diff>
--- a/frontend/translations/translations.xlsx
+++ b/frontend/translations/translations.xlsx
@@ -1,41 +1,182 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanvu/Library/Mobile Documents/com~apple~CloudDocs/Documents/Knowledge Hub/AI/Code/ht-catalyst/frontend/translations/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF84EABA-31EB-9741-8874-EF18132FC0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>vi</t>
+  </si>
+  <si>
+    <t>site.title</t>
+  </si>
+  <si>
+    <t>site.description</t>
+  </si>
+  <si>
+    <t>Discover insights on technology, personal growth, and making a positive impact</t>
+  </si>
+  <si>
+    <t>Khám phá những hiểu biết về công nghệ, phát triển bản thân và tạo tác động tích cực</t>
+  </si>
+  <si>
+    <t>nav.home</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Trang Chủ</t>
+  </si>
+  <si>
+    <t>nav.blog</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>nav.resources</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>Tài Nguyên</t>
+  </si>
+  <si>
+    <t>nav.about</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Giới Thiệu</t>
+  </si>
+  <si>
+    <t>hero.title</t>
+  </si>
+  <si>
+    <t>Welcome to My Knowledge Hub</t>
+  </si>
+  <si>
+    <t>Chào Mừng Đến Với Kho Kiến Thức</t>
+  </si>
+  <si>
+    <t>hero.subtitle</t>
+  </si>
+  <si>
+    <t>hero.description</t>
+  </si>
+  <si>
+    <t>Exploring the intersection of technology and social impact through thoughtful analysis and practical insights</t>
+  </si>
+  <si>
+    <t>Khám phá sự giao thoa giữa công nghệ và tác động xã hội thông qua phân tích sâu sắc và những hiểu biết thực tế</t>
+  </si>
+  <si>
+    <t>hero.cta.primary</t>
+  </si>
+  <si>
+    <t>Explore Resources</t>
+  </si>
+  <si>
+    <t>Khám Phá Tài Nguyên</t>
+  </si>
+  <si>
+    <t>hero.cta.secondary</t>
+  </si>
+  <si>
+    <t>View Blog</t>
+  </si>
+  <si>
+    <t>Xem Blog</t>
+  </si>
+  <si>
+    <t>newsletter.title</t>
+  </si>
+  <si>
+    <t>Subscribe to Newsletter</t>
+  </si>
+  <si>
+    <t>Đăng Ký Nhận Bản Tin</t>
+  </si>
+  <si>
+    <t>newsletter.description</t>
+  </si>
+  <si>
+    <t>Get the latest insights delivered to your inbox</t>
+  </si>
+  <si>
+    <t>Nhận những thông tin mới nhất qua email</t>
+  </si>
+  <si>
+    <t>newsletter.placeholder</t>
+  </si>
+  <si>
+    <t>Enter your email</t>
+  </si>
+  <si>
+    <t>Nhập email của bạn</t>
+  </si>
+  <si>
+    <t>newsletter.button</t>
+  </si>
+  <si>
+    <t>Subscribe</t>
+  </si>
+  <si>
+    <t>Đăng Ký</t>
+  </si>
+  <si>
+    <t>newsletter.success</t>
+  </si>
+  <si>
+    <t>Thank you for subscribing!</t>
+  </si>
+  <si>
+    <t>Cảm ơn bạn đã đăng ký!</t>
+  </si>
+  <si>
+    <t>newsletter.error</t>
+  </si>
+  <si>
+    <t>Something went wrong. Please try again.</t>
+  </si>
+  <si>
+    <t>Đã xảy ra lỗi. Vui lòng thử lại.</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +206,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,218 +545,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="50.83203125" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="2" max="3" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>key</v>
-      </c>
-      <c r="B1" t="str">
-        <v>en</v>
-      </c>
-      <c r="C1" t="str">
-        <v>vi</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>site.title</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Knowledge Hub</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Kho Kiến Thức</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>site.description</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Discover insights on technology, personal growth, and making a positive impact</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Khám phá những hiểu biết về công nghệ, phát triển bản thân và tạo tác động tích cực</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>nav.home</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Home</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Trang Chủ</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>nav.blog</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Blog</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Blog</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>nav.resources</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Resources</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Tài Nguyên</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>nav.about</v>
-      </c>
-      <c r="B7" t="str">
-        <v>About</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Giới Thiệu</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>hero.title</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Welcome to My Knowledge Hub</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Chào Mừng Đến Với Kho Kiến Thức</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>hero.subtitle</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Discover insights on technology, personal growth, and making a positive impact</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Khám phá những hiểu biết về công nghệ, phát triển bản thân và tạo tác động tích cực</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>hero.description</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Exploring the intersection of technology and social impact through thoughtful analysis and practical insights</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Khám phá sự giao thoa giữa công nghệ và tác động xã hội thông qua phân tích sâu sắc và những hiểu biết thực tế</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>hero.cta.primary</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Explore Resources</v>
-      </c>
-      <c r="C11" t="str">
-        <v>Khám Phá Tài Nguyên</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>hero.cta.secondary</v>
-      </c>
-      <c r="B12" t="str">
-        <v>View Blog</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Xem Blog</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>newsletter.title</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Subscribe to Newsletter</v>
-      </c>
-      <c r="C13" t="str">
-        <v>Đăng Ký Nhận Bản Tin</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>newsletter.description</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Get the latest insights delivered to your inbox</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Nhận những thông tin mới nhất qua email</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>newsletter.placeholder</v>
-      </c>
-      <c r="B15" t="str">
-        <v>Enter your email</v>
-      </c>
-      <c r="C15" t="str">
-        <v>Nhập email của bạn</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>newsletter.button</v>
-      </c>
-      <c r="B16" t="str">
-        <v>Subscribe</v>
-      </c>
-      <c r="C16" t="str">
-        <v>Đăng Ký</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>newsletter.success</v>
-      </c>
-      <c r="B17" t="str">
-        <v>Thank you for subscribing!</v>
-      </c>
-      <c r="C17" t="str">
-        <v>Cảm ơn bạn đã đăng ký!</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>newsletter.error</v>
-      </c>
-      <c r="B18" t="str">
-        <v>Something went wrong. Please try again.</v>
-      </c>
-      <c r="C18" t="str">
-        <v>Đã xảy ra lỗi. Vui lòng thử lại.</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C18"/>
+    <ignoredError sqref="A1:C1 A3:C18 A2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improve library, book details page, remove testing components
</commit_message>
<xml_diff>
--- a/frontend/translations/translations.xlsx
+++ b/frontend/translations/translations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -673,634 +673,766 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>blog.title</v>
+        <v>library.table_of_contents</v>
       </c>
       <c r="B25" t="str">
-        <v>Blog</v>
+        <v>Table of Contents</v>
       </c>
       <c r="C25" t="str">
-        <v>Blog</v>
+        <v>Mục Lục</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>blog.description</v>
+        <v>library.key_takeaways</v>
       </c>
       <c r="B26" t="str">
-        <v>Thoughts on product management, technology, and social impact</v>
+        <v>Key Takeaways</v>
       </c>
       <c r="C26" t="str">
-        <v>Suy nghĩ về quản lý sản phẩm, công nghệ và tác động xã hội</v>
+        <v>Điểm Chính</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>blog.read_more</v>
+        <v>library.book_not_found</v>
       </c>
       <c r="B27" t="str">
-        <v>Read More</v>
+        <v>Book not found</v>
       </c>
       <c r="C27" t="str">
-        <v>Đọc Thêm</v>
+        <v>Không tìm thấy sách</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>blog.latest_posts</v>
+        <v>library.book_not_found_description</v>
       </c>
       <c r="B28" t="str">
-        <v>Latest Posts</v>
+        <v>Sorry, we couldn't find the book you're looking for.</v>
       </c>
       <c r="C28" t="str">
-        <v>Bài Viết Mới Nhất</v>
+        <v>Xin lỗi, chúng tôi không thể tìm thấy cuốn sách bạn đang tìm kiếm.</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>blog.no_posts_title</v>
+        <v>library.reading_time</v>
       </c>
       <c r="B29" t="str">
-        <v>No Posts Yet</v>
+        <v>{{minutes}} min read</v>
       </c>
       <c r="C29" t="str">
-        <v>Chưa Có Bài Viết</v>
+        <v>{{minutes}} phút đọc</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>blog.no_posts_description</v>
+        <v>library.chapter</v>
       </c>
       <c r="B30" t="str">
-        <v>Check back soon for new content!</v>
+        <v>Chapter {{number}}</v>
       </c>
       <c r="C30" t="str">
-        <v>Vui lòng quay lại sau để xem nội dung mới!</v>
+        <v>Chương {{number}}</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>resources.title</v>
+        <v>library.previous_chapter</v>
       </c>
       <c r="B31" t="str">
-        <v>Resources</v>
+        <v>Previous Chapter</v>
       </c>
       <c r="C31" t="str">
-        <v>Tài Nguyên</v>
+        <v>Chương Trước</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>resources.description</v>
+        <v>library.next_chapter</v>
       </c>
       <c r="B32" t="str">
-        <v>A collection of tools, guides, and resources to help you on your journey</v>
+        <v>Next Chapter</v>
       </c>
       <c r="C32" t="str">
-        <v>Bộ sưu tập công cụ, hướng dẫn và tài nguyên để hỗ trợ bạn trên hành trình của mình</v>
+        <v>Chương Tiếp Theo</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>resources.tools</v>
+        <v>library.by</v>
       </c>
       <c r="B33" t="str">
-        <v>Tools</v>
+        <v>by</v>
       </c>
       <c r="C33" t="str">
-        <v>Công Cụ</v>
+        <v>bởi</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>resources.guides</v>
+        <v>library.last_updated</v>
       </c>
       <c r="B34" t="str">
-        <v>Guides</v>
+        <v>Last updated {{date}}</v>
       </c>
       <c r="C34" t="str">
-        <v>Hướng Dẫn</v>
+        <v>Cập nhật lần cuối {{date}}</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>about.title</v>
+        <v>blog.title</v>
       </c>
       <c r="B35" t="str">
-        <v>About Me</v>
+        <v>Blog</v>
       </c>
       <c r="C35" t="str">
-        <v>Về Tôi</v>
+        <v>Blog</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>about.intro</v>
+        <v>blog.description</v>
       </c>
       <c r="B36" t="str">
-        <v>Hi, I'm Jonathan. I'm passionate about technology and making a positive impact.</v>
+        <v>Thoughts on product management, technology, and social impact</v>
       </c>
       <c r="C36" t="str">
-        <v>Xin chào, tôi là Jonathan. Tôi đam mê công nghệ và tạo ra những tác động tích cực.</v>
+        <v>Suy nghĩ về quản lý sản phẩm, công nghệ và tác động xã hội</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>about.mission</v>
+        <v>blog.read_more</v>
       </c>
       <c r="B37" t="str">
-        <v>My mission is to help others leverage technology for positive change.</v>
+        <v>Read More</v>
       </c>
       <c r="C37" t="str">
-        <v>Sứ mệnh của tôi là giúp mọi người tận dụng công nghệ để tạo ra những thay đổi tích cực.</v>
+        <v>Đọc Thêm</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>about.contact</v>
+        <v>blog.latest_posts</v>
       </c>
       <c r="B38" t="str">
-        <v>Get in Touch</v>
+        <v>Latest Posts</v>
       </c>
       <c r="C38" t="str">
-        <v>Liên Hệ</v>
+        <v>Bài Viết Mới Nhất</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>about.background.title</v>
+        <v>blog.no_posts_title</v>
       </c>
       <c r="B39" t="str">
-        <v>Background</v>
+        <v>No Posts Yet</v>
       </c>
       <c r="C39" t="str">
-        <v>Giới Thiệu</v>
+        <v>Chưa Có Bài Viết</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>about.background.content</v>
+        <v>blog.no_posts_description</v>
       </c>
       <c r="B40" t="str">
-        <v>As a Product Manager with a passion for technology and social impact, I bridge the gap between innovative solutions and human needs. My journey in product management has been driven by a commitment to creating meaningful digital experiences that make a difference.</v>
+        <v>Check back soon for new content!</v>
       </c>
       <c r="C40" t="str">
-        <v>Là một Product Manager với niềm đam mê về công nghệ và tác động xã hội, tôi kết nối giữa các giải pháp sáng tạo và nhu cầu con người. Hành trình của tôi trong quản lý sản phẩm được thúc đẩy bởi cam kết tạo ra những trải nghiệm kỹ thuật số có ý nghĩa.</v>
+        <v>Vui lòng quay lại sau để xem nội dung mới!</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>about.expertise.title</v>
+        <v>resources.title</v>
       </c>
       <c r="B41" t="str">
-        <v>Expertise</v>
+        <v>Resources</v>
       </c>
       <c r="C41" t="str">
-        <v>Chuyên Môn</v>
+        <v>Tài Nguyên</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>about.expertise.skills.product_strategy</v>
+        <v>resources.description</v>
       </c>
       <c r="B42" t="str">
-        <v>Product Strategy</v>
+        <v>A collection of tools, guides, and resources to help you on your journey</v>
       </c>
       <c r="C42" t="str">
-        <v>Chiến Lược Sản Phẩm</v>
+        <v>Bộ sưu tập công cụ, hướng dẫn và tài nguyên để hỗ trợ bạn trên hành trình của mình</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>about.expertise.skills.user_research</v>
+        <v>resources.tools</v>
       </c>
       <c r="B43" t="str">
-        <v>User Research</v>
+        <v>Tools</v>
       </c>
       <c r="C43" t="str">
-        <v>Nghiên Cứu Người Dùng</v>
+        <v>Công Cụ</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>about.expertise.skills.agile</v>
+        <v>resources.guides</v>
       </c>
       <c r="B44" t="str">
-        <v>Agile Management</v>
+        <v>Guides</v>
       </c>
       <c r="C44" t="str">
-        <v>Quản Lý Agile</v>
+        <v>Hướng Dẫn</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>about.expertise.skills.analytics</v>
+        <v>about.title</v>
       </c>
       <c r="B45" t="str">
-        <v>Data Analytics</v>
+        <v>About Me</v>
       </c>
       <c r="C45" t="str">
-        <v>Phân Tích Dữ Liệu</v>
+        <v>Về Tôi</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>about.expertise.skills.technical</v>
+        <v>about.intro</v>
       </c>
       <c r="B46" t="str">
-        <v>Technical Leadership</v>
+        <v>Hi, I'm Jonathan. I'm passionate about technology and making a positive impact.</v>
       </c>
       <c r="C46" t="str">
-        <v>Lãnh Đạo Kỹ Thuật</v>
+        <v>Xin chào, tôi là Jonathan. Tôi đam mê công nghệ và tạo ra những tác động tích cực.</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>about.vision.title</v>
+        <v>about.mission</v>
       </c>
       <c r="B47" t="str">
-        <v>Vision</v>
+        <v>My mission is to help others leverage technology for positive change.</v>
       </c>
       <c r="C47" t="str">
-        <v>Tầm Nhìn</v>
+        <v>Sứ mệnh của tôi là giúp mọi người tận dụng công nghệ để tạo ra những thay đổi tích cực.</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>about.vision.content</v>
+        <v>about.contact</v>
       </c>
       <c r="B48" t="str">
-        <v>I believe in leveraging technology to create products that not only solve problems but also contribute positively to society. My goal is to lead product initiatives that combine innovation with social responsibility.</v>
+        <v>Get in Touch</v>
       </c>
       <c r="C48" t="str">
-        <v>Tôi tin vào việc tận dụng công nghệ để tạo ra những sản phẩm không chỉ giải quyết vấn đề mà còn đóng góp tích cực cho xã hội. Mục tiêu của tôi là dẫn dắt các sáng kiến sản phẩm kết hợp đổi mới với trách nhiệm xã hội.</v>
+        <v>Liên Hệ</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>about.timeline.present.year</v>
+        <v>about.background.title</v>
       </c>
       <c r="B49" t="str">
-        <v>2023 - Present</v>
+        <v>Background</v>
       </c>
       <c r="C49" t="str">
-        <v>2023 - Hiện tại</v>
+        <v>Giới Thiệu</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>about.timeline.present.title</v>
+        <v>about.background.content</v>
       </c>
       <c r="B50" t="str">
-        <v>Senior Product Manager</v>
+        <v>As a Product Manager with a passion for technology and social impact, I bridge the gap between innovative solutions and human needs. My journey in product management has been driven by a commitment to creating meaningful digital experiences that make a difference.</v>
       </c>
       <c r="C50" t="str">
-        <v>Quản Lý Sản Phẩm Cao Cấp</v>
+        <v>Là một Product Manager với niềm đam mê về công nghệ và tác động xã hội, tôi kết nối giữa các giải pháp sáng tạo và nhu cầu con người. Hành trình của tôi trong quản lý sản phẩm được thúc đẩy bởi cam kết tạo ra những trải nghiệm kỹ thuật số có ý nghĩa.</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>about.timeline.present.description</v>
+        <v>about.expertise.title</v>
       </c>
       <c r="B51" t="str">
-        <v>Leading innovative product initiatives</v>
+        <v>Expertise</v>
       </c>
       <c r="C51" t="str">
-        <v>Dẫn dắt các sáng kiến sản phẩm sáng tạo</v>
+        <v>Chuyên Môn</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>about.timeline.past_1.year</v>
+        <v>about.expertise.skills.product_strategy</v>
       </c>
       <c r="B52" t="str">
-        <v>2020 - 2023</v>
+        <v>Product Strategy</v>
       </c>
       <c r="C52" t="str">
-        <v>2020 - 2023</v>
+        <v>Chiến Lược Sản Phẩm</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>about.timeline.past_1.title</v>
+        <v>about.expertise.skills.user_research</v>
       </c>
       <c r="B53" t="str">
-        <v>Product Manager</v>
+        <v>User Research</v>
       </c>
       <c r="C53" t="str">
-        <v>Quản Lý Sản Phẩm</v>
+        <v>Nghiên Cứu Người Dùng</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>about.timeline.past_1.description</v>
+        <v>about.expertise.skills.agile</v>
       </c>
       <c r="B54" t="str">
-        <v>Driving user-centered product development</v>
+        <v>Agile Management</v>
       </c>
       <c r="C54" t="str">
-        <v>Thúc đẩy phát triển sản phẩm lấy người dùng làm trung tâm</v>
+        <v>Quản Lý Agile</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>about.timeline.past_2.year</v>
+        <v>about.expertise.skills.analytics</v>
       </c>
       <c r="B55" t="str">
-        <v>2018 - 2020</v>
+        <v>Data Analytics</v>
       </c>
       <c r="C55" t="str">
-        <v>2018 - 2020</v>
+        <v>Phân Tích Dữ Liệu</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>about.timeline.past_2.title</v>
+        <v>about.expertise.skills.technical</v>
       </c>
       <c r="B56" t="str">
-        <v>Associate Product Manager</v>
+        <v>Technical Leadership</v>
       </c>
       <c r="C56" t="str">
-        <v>Quản Lý Sản Phẩm Phó</v>
+        <v>Lãnh Đạo Kỹ Thuật</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>about.timeline.past_2.description</v>
+        <v>about.vision.title</v>
       </c>
       <c r="B57" t="str">
-        <v>Building foundation in product management</v>
+        <v>Vision</v>
       </c>
       <c r="C57" t="str">
-        <v>Xây dựng nền tảng trong quản lý sản phẩm</v>
+        <v>Tầm Nhìn</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>contact.title</v>
+        <v>about.vision.content</v>
       </c>
       <c r="B58" t="str">
-        <v>Get in Touch</v>
+        <v>I believe in leveraging technology to create products that not only solve problems but also contribute positively to society. My goal is to lead product initiatives that combine innovation with social responsibility.</v>
       </c>
       <c r="C58" t="str">
-        <v>Get in Touch</v>
+        <v>Tôi tin vào việc tận dụng công nghệ để tạo ra những sản phẩm không chỉ giải quyết vấn đề mà còn đóng góp tích cực cho xã hội. Mục tiêu của tôi là dẫn dắt các sáng kiến sản phẩm kết hợp đổi mới với trách nhiệm xã hội.</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>contact.description</v>
+        <v>about.timeline.present.year</v>
       </c>
       <c r="B59" t="str">
-        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
+        <v>2023 - Present</v>
       </c>
       <c r="C59" t="str">
-        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
+        <v>2023 - Hiện tại</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>contact.form.name</v>
+        <v>about.timeline.present.title</v>
       </c>
       <c r="B60" t="str">
-        <v>Your Name</v>
+        <v>Senior Product Manager</v>
       </c>
       <c r="C60" t="str">
-        <v>Your Name</v>
+        <v>Quản Lý Sản Phẩm Cao Cấp</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>contact.form.email</v>
+        <v>about.timeline.present.description</v>
       </c>
       <c r="B61" t="str">
-        <v>Your Email</v>
+        <v>Leading innovative product initiatives</v>
       </c>
       <c r="C61" t="str">
-        <v>Your Email</v>
+        <v>Dẫn dắt các sáng kiến sản phẩm sáng tạo</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>contact.form.message</v>
+        <v>about.timeline.past_1.year</v>
       </c>
       <c r="B62" t="str">
-        <v>Your Message</v>
+        <v>2020 - 2023</v>
       </c>
       <c r="C62" t="str">
-        <v>Your Message</v>
+        <v>2020 - 2023</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>contact.form.submit</v>
+        <v>about.timeline.past_1.title</v>
       </c>
       <c r="B63" t="str">
-        <v>Send Message</v>
+        <v>Product Manager</v>
       </c>
       <c r="C63" t="str">
-        <v>Send Message</v>
+        <v>Quản Lý Sản Phẩm</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>contact.form.success</v>
+        <v>about.timeline.past_1.description</v>
       </c>
       <c r="B64" t="str">
-        <v>Message sent successfully!</v>
+        <v>Driving user-centered product development</v>
       </c>
       <c r="C64" t="str">
-        <v>Message sent successfully!</v>
+        <v>Thúc đẩy phát triển sản phẩm lấy người dùng làm trung tâm</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>contact.form.error</v>
+        <v>about.timeline.past_2.year</v>
       </c>
       <c r="B65" t="str">
-        <v>Error sending message. Please try again.</v>
+        <v>2018 - 2020</v>
       </c>
       <c r="C65" t="str">
-        <v>Error sending message. Please try again.</v>
+        <v>2018 - 2020</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>finance.title</v>
+        <v>about.timeline.past_2.title</v>
       </c>
       <c r="B66" t="str">
-        <v>Personal Finance</v>
+        <v>Associate Product Manager</v>
       </c>
       <c r="C66" t="str">
-        <v>Quản Lý Tài Chính Cá Nhân</v>
+        <v>Quản Lý Sản Phẩm Phó</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>finance.description</v>
+        <v>about.timeline.past_2.description</v>
       </c>
       <c r="B67" t="str">
-        <v>Insights and strategies for building financial independence</v>
+        <v>Building foundation in product management</v>
       </c>
       <c r="C67" t="str">
-        <v>Những hiểu biết và chiến lược để xây dựng tự do tài chính</v>
+        <v>Xây dựng nền tảng trong quản lý sản phẩm</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>finance.sections.investments.title</v>
+        <v>contact.title</v>
       </c>
       <c r="B68" t="str">
-        <v>Investment Strategies</v>
+        <v>Get in Touch</v>
       </c>
       <c r="C68" t="str">
-        <v>Chiến Lược Đầu Tư</v>
+        <v>Get in Touch</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>finance.sections.investments.description</v>
+        <v>contact.description</v>
       </c>
       <c r="B69" t="str">
-        <v>Long-term approaches to wealth building</v>
+        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
       </c>
       <c r="C69" t="str">
-        <v>Phương pháp xây dựng tài sản dài hạn</v>
+        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>finance.sections.budgeting.title</v>
+        <v>contact.form.name</v>
       </c>
       <c r="B70" t="str">
-        <v>Smart Budgeting</v>
+        <v>Your Name</v>
       </c>
       <c r="C70" t="str">
-        <v>Quản Lý Chi Tiêu</v>
+        <v>Your Name</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>finance.sections.budgeting.description</v>
+        <v>contact.form.email</v>
       </c>
       <c r="B71" t="str">
-        <v>Practical tips for effective money management</v>
+        <v>Your Email</v>
       </c>
       <c r="C71" t="str">
-        <v>Mẹo thực tế để quản lý tiền hiệu quả</v>
+        <v>Your Email</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>finance.sections.planning.title</v>
+        <v>contact.form.message</v>
       </c>
       <c r="B72" t="str">
-        <v>Financial Planning</v>
+        <v>Your Message</v>
       </c>
       <c r="C72" t="str">
-        <v>Kế Hoạch Tài Chính</v>
+        <v>Your Message</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>finance.sections.planning.description</v>
+        <v>contact.form.submit</v>
       </c>
       <c r="B73" t="str">
-        <v>Setting and achieving financial goals</v>
+        <v>Send Message</v>
       </c>
       <c r="C73" t="str">
-        <v>Thiết lập và đạt được mục tiêu tài chính</v>
+        <v>Send Message</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>impact.title</v>
+        <v>contact.form.success</v>
       </c>
       <c r="B74" t="str">
-        <v>Social Impact</v>
+        <v>Message sent successfully!</v>
       </c>
       <c r="C74" t="str">
-        <v>Tác Động Xã Hội</v>
+        <v>Message sent successfully!</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>impact.description</v>
+        <v>contact.form.error</v>
       </c>
       <c r="B75" t="str">
-        <v>Making a positive difference in the world</v>
+        <v>Error sending message. Please try again.</v>
       </c>
       <c r="C75" t="str">
-        <v>Tạo ra những thay đổi tích cực cho thế giới</v>
+        <v>Error sending message. Please try again.</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>impact.sections.projects.title</v>
+        <v>finance.title</v>
       </c>
       <c r="B76" t="str">
-        <v>Impact Projects</v>
+        <v>Personal Finance</v>
       </c>
       <c r="C76" t="str">
-        <v>Dự Án Tác Động</v>
+        <v>Quản Lý Tài Chính Cá Nhân</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>impact.sections.projects.description</v>
+        <v>finance.description</v>
       </c>
       <c r="B77" t="str">
-        <v>Current initiatives and their outcomes</v>
+        <v>Insights and strategies for building financial independence</v>
       </c>
       <c r="C77" t="str">
-        <v>Các sáng kiến hiện tại và kết quả</v>
+        <v>Những hiểu biết và chiến lược để xây dựng tự do tài chính</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>impact.sections.metrics.title</v>
+        <v>finance.sections.investments.title</v>
       </c>
       <c r="B78" t="str">
-        <v>Impact Metrics</v>
+        <v>Investment Strategies</v>
       </c>
       <c r="C78" t="str">
-        <v>Đo Lường Tác Động</v>
+        <v>Chiến Lược Đầu Tư</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>impact.sections.metrics.description</v>
+        <v>finance.sections.investments.description</v>
       </c>
       <c r="B79" t="str">
-        <v>Measuring and tracking social impact</v>
+        <v>Long-term approaches to wealth building</v>
       </c>
       <c r="C79" t="str">
-        <v>Đo lường và theo dõi tác động xã hội</v>
+        <v>Phương pháp xây dựng tài sản dài hạn</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>impact.sections.collaboration.title</v>
+        <v>finance.sections.budgeting.title</v>
       </c>
       <c r="B80" t="str">
-        <v>Get Involved</v>
+        <v>Smart Budgeting</v>
       </c>
       <c r="C80" t="str">
-        <v>Tham Gia</v>
+        <v>Quản Lý Chi Tiêu</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
+        <v>finance.sections.budgeting.description</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Practical tips for effective money management</v>
+      </c>
+      <c r="C81" t="str">
+        <v>Mẹo thực tế để quản lý tiền hiệu quả</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>finance.sections.planning.title</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Financial Planning</v>
+      </c>
+      <c r="C82" t="str">
+        <v>Kế Hoạch Tài Chính</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>finance.sections.planning.description</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Setting and achieving financial goals</v>
+      </c>
+      <c r="C83" t="str">
+        <v>Thiết lập và đạt được mục tiêu tài chính</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>impact.title</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Social Impact</v>
+      </c>
+      <c r="C84" t="str">
+        <v>Tác Động Xã Hội</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>impact.description</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Making a positive difference in the world</v>
+      </c>
+      <c r="C85" t="str">
+        <v>Tạo ra những thay đổi tích cực cho thế giới</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>impact.sections.projects.title</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Impact Projects</v>
+      </c>
+      <c r="C86" t="str">
+        <v>Dự Án Tác Động</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>impact.sections.projects.description</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Current initiatives and their outcomes</v>
+      </c>
+      <c r="C87" t="str">
+        <v>Các sáng kiến hiện tại và kết quả</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>impact.sections.metrics.title</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Impact Metrics</v>
+      </c>
+      <c r="C88" t="str">
+        <v>Đo Lường Tác Động</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>impact.sections.metrics.description</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Measuring and tracking social impact</v>
+      </c>
+      <c r="C89" t="str">
+        <v>Đo lường và theo dõi tác động xã hội</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>impact.sections.collaboration.title</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Get Involved</v>
+      </c>
+      <c r="C90" t="str">
+        <v>Tham Gia</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
         <v>impact.sections.collaboration.description</v>
       </c>
-      <c r="B81" t="str">
+      <c r="B91" t="str">
         <v>Ways to contribute and collaborate</v>
       </c>
-      <c r="C81" t="str">
+      <c r="C91" t="str">
         <v>Cách đóng góp và hợp tác</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>common.back_to_library</v>
+      </c>
+      <c r="B92" t="str">
+        <v>Back to Library</v>
+      </c>
+      <c r="C92" t="str">
+        <v>Quay Lại Thư Viện</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>common.published_on</v>
+      </c>
+      <c r="B93" t="str">
+        <v>Published on {{date}}</v>
+      </c>
+      <c r="C93" t="str">
+        <v>Xuất bản ngày {{date}}</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C81"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C93"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final check the translations and dark mode
</commit_message>
<xml_diff>
--- a/frontend/translations/translations.xlsx
+++ b/frontend/translations/translations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -849,590 +849,656 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>resources.title</v>
+        <v>blog.categories.all</v>
       </c>
       <c r="B41" t="str">
-        <v>Resources</v>
+        <v>All Posts</v>
       </c>
       <c r="C41" t="str">
-        <v>Tài Nguyên</v>
+        <v>Tất Cả Bài Viết</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>resources.description</v>
+        <v>blog.categories.product</v>
       </c>
       <c r="B42" t="str">
-        <v>A collection of tools, guides, and resources to help you on your journey</v>
+        <v>Product Management</v>
       </c>
       <c r="C42" t="str">
-        <v>Bộ sưu tập công cụ, hướng dẫn và tài nguyên để hỗ trợ bạn trên hành trình của mình</v>
+        <v>Quản Lý Sản Phẩm</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>resources.tools</v>
+        <v>blog.categories.impact</v>
       </c>
       <c r="B43" t="str">
-        <v>Tools</v>
+        <v>Social Impact</v>
       </c>
       <c r="C43" t="str">
-        <v>Công Cụ</v>
+        <v>Tác Động Xã Hội</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>resources.guides</v>
+        <v>blog.categories.projects</v>
       </c>
       <c r="B44" t="str">
-        <v>Guides</v>
+        <v>Side Projects</v>
       </c>
       <c r="C44" t="str">
-        <v>Hướng Dẫn</v>
+        <v>Dự Án Cá Nhân</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>about.title</v>
+        <v>blog.categories.family</v>
       </c>
       <c r="B45" t="str">
-        <v>About Me</v>
+        <v>Family</v>
       </c>
       <c r="C45" t="str">
-        <v>Về Tôi</v>
+        <v>Gia Đình</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>about.intro</v>
+        <v>blog.categories.growth</v>
       </c>
       <c r="B46" t="str">
-        <v>Hi, I'm Jonathan. I'm passionate about technology and making a positive impact.</v>
+        <v>Personal Growth</v>
       </c>
       <c r="C46" t="str">
-        <v>Xin chào, tôi là Jonathan. Tôi đam mê công nghệ và tạo ra những tác động tích cực.</v>
+        <v>Phát Triển Bản Thân</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>about.mission</v>
+        <v>resources.title</v>
       </c>
       <c r="B47" t="str">
-        <v>My mission is to help others leverage technology for positive change.</v>
+        <v>Resources</v>
       </c>
       <c r="C47" t="str">
-        <v>Sứ mệnh của tôi là giúp mọi người tận dụng công nghệ để tạo ra những thay đổi tích cực.</v>
+        <v>Tài Nguyên</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>about.contact</v>
+        <v>resources.description</v>
       </c>
       <c r="B48" t="str">
-        <v>Get in Touch</v>
+        <v>A collection of tools, guides, and resources to help you on your journey</v>
       </c>
       <c r="C48" t="str">
-        <v>Liên Hệ</v>
+        <v>Bộ sưu tập công cụ, hướng dẫn và tài nguyên để hỗ trợ bạn trên hành trình của mình</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>about.background.title</v>
+        <v>resources.tools</v>
       </c>
       <c r="B49" t="str">
-        <v>Background</v>
+        <v>Tools</v>
       </c>
       <c r="C49" t="str">
-        <v>Giới Thiệu</v>
+        <v>Công Cụ</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>about.background.content</v>
+        <v>resources.guides</v>
       </c>
       <c r="B50" t="str">
-        <v>As a Product Manager with a passion for technology and social impact, I bridge the gap between innovative solutions and human needs. My journey in product management has been driven by a commitment to creating meaningful digital experiences that make a difference.</v>
+        <v>Guides</v>
       </c>
       <c r="C50" t="str">
-        <v>Là một Product Manager với niềm đam mê về công nghệ và tác động xã hội, tôi kết nối giữa các giải pháp sáng tạo và nhu cầu con người. Hành trình của tôi trong quản lý sản phẩm được thúc đẩy bởi cam kết tạo ra những trải nghiệm kỹ thuật số có ý nghĩa.</v>
+        <v>Hướng Dẫn</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>about.expertise.title</v>
+        <v>about.title</v>
       </c>
       <c r="B51" t="str">
-        <v>Expertise</v>
+        <v>About Me</v>
       </c>
       <c r="C51" t="str">
-        <v>Chuyên Môn</v>
+        <v>Về Tôi</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>about.expertise.skills.product_strategy</v>
+        <v>about.intro</v>
       </c>
       <c r="B52" t="str">
-        <v>Product Strategy</v>
+        <v>Hi, I'm Jonathan. I'm passionate about technology and making a positive impact.</v>
       </c>
       <c r="C52" t="str">
-        <v>Chiến Lược Sản Phẩm</v>
+        <v>Xin chào, tôi là Jonathan. Tôi đam mê công nghệ và tạo ra những tác động tích cực.</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>about.expertise.skills.user_research</v>
+        <v>about.mission</v>
       </c>
       <c r="B53" t="str">
-        <v>User Research</v>
+        <v>My mission is to help others leverage technology for positive change.</v>
       </c>
       <c r="C53" t="str">
-        <v>Nghiên Cứu Người Dùng</v>
+        <v>Sứ mệnh của tôi là giúp mọi người tận dụng công nghệ để tạo ra những thay đổi tích cực.</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>about.expertise.skills.agile</v>
+        <v>about.contact</v>
       </c>
       <c r="B54" t="str">
-        <v>Agile Management</v>
+        <v>Get in Touch</v>
       </c>
       <c r="C54" t="str">
-        <v>Quản Lý Agile</v>
+        <v>Liên Hệ</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>about.expertise.skills.analytics</v>
+        <v>about.background.title</v>
       </c>
       <c r="B55" t="str">
-        <v>Data Analytics</v>
+        <v>Background</v>
       </c>
       <c r="C55" t="str">
-        <v>Phân Tích Dữ Liệu</v>
+        <v>Giới Thiệu</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>about.expertise.skills.technical</v>
+        <v>about.background.content</v>
       </c>
       <c r="B56" t="str">
-        <v>Technical Leadership</v>
+        <v>As a Product Manager with a passion for technology and social impact, I bridge the gap between innovative solutions and human needs. My journey in product management has been driven by a commitment to creating meaningful digital experiences that make a difference.</v>
       </c>
       <c r="C56" t="str">
-        <v>Lãnh Đạo Kỹ Thuật</v>
+        <v>Là một Product Manager với niềm đam mê về công nghệ và tác động xã hội, tôi kết nối giữa các giải pháp sáng tạo và nhu cầu con người. Hành trình của tôi trong quản lý sản phẩm được thúc đẩy bởi cam kết tạo ra những trải nghiệm kỹ thuật số có ý nghĩa.</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>about.vision.title</v>
+        <v>about.expertise.title</v>
       </c>
       <c r="B57" t="str">
-        <v>Vision</v>
+        <v>Expertise</v>
       </c>
       <c r="C57" t="str">
-        <v>Tầm Nhìn</v>
+        <v>Chuyên Môn</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>about.vision.content</v>
+        <v>about.expertise.skills.product_strategy</v>
       </c>
       <c r="B58" t="str">
-        <v>I believe in leveraging technology to create products that not only solve problems but also contribute positively to society. My goal is to lead product initiatives that combine innovation with social responsibility.</v>
+        <v>Product Strategy</v>
       </c>
       <c r="C58" t="str">
-        <v>Tôi tin vào việc tận dụng công nghệ để tạo ra những sản phẩm không chỉ giải quyết vấn đề mà còn đóng góp tích cực cho xã hội. Mục tiêu của tôi là dẫn dắt các sáng kiến sản phẩm kết hợp đổi mới với trách nhiệm xã hội.</v>
+        <v>Chiến Lược Sản Phẩm</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>about.timeline.present.year</v>
+        <v>about.expertise.skills.user_research</v>
       </c>
       <c r="B59" t="str">
-        <v>2023 - Present</v>
+        <v>User Research</v>
       </c>
       <c r="C59" t="str">
-        <v>2023 - Hiện tại</v>
+        <v>Nghiên Cứu Người Dùng</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>about.timeline.present.title</v>
+        <v>about.expertise.skills.agile</v>
       </c>
       <c r="B60" t="str">
-        <v>Senior Product Manager</v>
+        <v>Agile Management</v>
       </c>
       <c r="C60" t="str">
-        <v>Quản Lý Sản Phẩm Cao Cấp</v>
+        <v>Quản Lý Agile</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>about.timeline.present.description</v>
+        <v>about.expertise.skills.analytics</v>
       </c>
       <c r="B61" t="str">
-        <v>Leading innovative product initiatives</v>
+        <v>Data Analytics</v>
       </c>
       <c r="C61" t="str">
-        <v>Dẫn dắt các sáng kiến sản phẩm sáng tạo</v>
+        <v>Phân Tích Dữ Liệu</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>about.timeline.past_1.year</v>
+        <v>about.expertise.skills.technical</v>
       </c>
       <c r="B62" t="str">
-        <v>2020 - 2023</v>
+        <v>Technical Leadership</v>
       </c>
       <c r="C62" t="str">
-        <v>2020 - 2023</v>
+        <v>Lãnh Đạo Kỹ Thuật</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>about.timeline.past_1.title</v>
+        <v>about.vision.title</v>
       </c>
       <c r="B63" t="str">
-        <v>Product Manager</v>
+        <v>Vision</v>
       </c>
       <c r="C63" t="str">
-        <v>Quản Lý Sản Phẩm</v>
+        <v>Tầm Nhìn</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>about.timeline.past_1.description</v>
+        <v>about.vision.content</v>
       </c>
       <c r="B64" t="str">
-        <v>Driving user-centered product development</v>
+        <v>I believe in leveraging technology to create products that not only solve problems but also contribute positively to society. My goal is to lead product initiatives that combine innovation with social responsibility.</v>
       </c>
       <c r="C64" t="str">
-        <v>Thúc đẩy phát triển sản phẩm lấy người dùng làm trung tâm</v>
+        <v>Tôi tin vào việc tận dụng công nghệ để tạo ra những sản phẩm không chỉ giải quyết vấn đề mà còn đóng góp tích cực cho xã hội. Mục tiêu của tôi là dẫn dắt các sáng kiến sản phẩm kết hợp đổi mới với trách nhiệm xã hội.</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>about.timeline.past_2.year</v>
+        <v>about.timeline.present.year</v>
       </c>
       <c r="B65" t="str">
-        <v>2018 - 2020</v>
+        <v>2023 - Present</v>
       </c>
       <c r="C65" t="str">
-        <v>2018 - 2020</v>
+        <v>2023 - Hiện tại</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>about.timeline.past_2.title</v>
+        <v>about.timeline.present.title</v>
       </c>
       <c r="B66" t="str">
-        <v>Associate Product Manager</v>
+        <v>Senior Product Manager</v>
       </c>
       <c r="C66" t="str">
-        <v>Quản Lý Sản Phẩm Phó</v>
+        <v>Quản Lý Sản Phẩm Cao Cấp</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>about.timeline.past_2.description</v>
+        <v>about.timeline.present.description</v>
       </c>
       <c r="B67" t="str">
-        <v>Building foundation in product management</v>
+        <v>Leading innovative product initiatives</v>
       </c>
       <c r="C67" t="str">
-        <v>Xây dựng nền tảng trong quản lý sản phẩm</v>
+        <v>Dẫn dắt các sáng kiến sản phẩm sáng tạo</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>contact.title</v>
+        <v>about.timeline.past_1.year</v>
       </c>
       <c r="B68" t="str">
-        <v>Get in Touch</v>
+        <v>2020 - 2023</v>
       </c>
       <c r="C68" t="str">
-        <v>Get in Touch</v>
+        <v>2020 - 2023</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>contact.description</v>
+        <v>about.timeline.past_1.title</v>
       </c>
       <c r="B69" t="str">
-        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
+        <v>Product Manager</v>
       </c>
       <c r="C69" t="str">
-        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
+        <v>Quản Lý Sản Phẩm</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>contact.form.name</v>
+        <v>about.timeline.past_1.description</v>
       </c>
       <c r="B70" t="str">
-        <v>Your Name</v>
+        <v>Driving user-centered product development</v>
       </c>
       <c r="C70" t="str">
-        <v>Your Name</v>
+        <v>Thúc đẩy phát triển sản phẩm lấy người dùng làm trung tâm</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>contact.form.email</v>
+        <v>about.timeline.past_2.year</v>
       </c>
       <c r="B71" t="str">
-        <v>Your Email</v>
+        <v>2018 - 2020</v>
       </c>
       <c r="C71" t="str">
-        <v>Your Email</v>
+        <v>2018 - 2020</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>contact.form.message</v>
+        <v>about.timeline.past_2.title</v>
       </c>
       <c r="B72" t="str">
-        <v>Your Message</v>
+        <v>Associate Product Manager</v>
       </c>
       <c r="C72" t="str">
-        <v>Your Message</v>
+        <v>Quản Lý Sản Phẩm Phó</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>contact.form.submit</v>
+        <v>about.timeline.past_2.description</v>
       </c>
       <c r="B73" t="str">
-        <v>Send Message</v>
+        <v>Building foundation in product management</v>
       </c>
       <c r="C73" t="str">
-        <v>Send Message</v>
+        <v>Xây dựng nền tảng trong quản lý sản phẩm</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>contact.form.success</v>
+        <v>contact.title</v>
       </c>
       <c r="B74" t="str">
-        <v>Message sent successfully!</v>
+        <v>Get in Touch</v>
       </c>
       <c r="C74" t="str">
-        <v>Message sent successfully!</v>
+        <v>Get in Touch</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>contact.form.error</v>
+        <v>contact.description</v>
       </c>
       <c r="B75" t="str">
-        <v>Error sending message. Please try again.</v>
+        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
       </c>
       <c r="C75" t="str">
-        <v>Error sending message. Please try again.</v>
+        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>finance.title</v>
+        <v>contact.form.name</v>
       </c>
       <c r="B76" t="str">
-        <v>Personal Finance</v>
+        <v>Your Name</v>
       </c>
       <c r="C76" t="str">
-        <v>Quản Lý Tài Chính Cá Nhân</v>
+        <v>Your Name</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>finance.description</v>
+        <v>contact.form.email</v>
       </c>
       <c r="B77" t="str">
-        <v>Insights and strategies for building financial independence</v>
+        <v>Your Email</v>
       </c>
       <c r="C77" t="str">
-        <v>Những hiểu biết và chiến lược để xây dựng tự do tài chính</v>
+        <v>Your Email</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>finance.sections.investments.title</v>
+        <v>contact.form.message</v>
       </c>
       <c r="B78" t="str">
-        <v>Investment Strategies</v>
+        <v>Your Message</v>
       </c>
       <c r="C78" t="str">
-        <v>Chiến Lược Đầu Tư</v>
+        <v>Your Message</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>finance.sections.investments.description</v>
+        <v>contact.form.submit</v>
       </c>
       <c r="B79" t="str">
-        <v>Long-term approaches to wealth building</v>
+        <v>Send Message</v>
       </c>
       <c r="C79" t="str">
-        <v>Phương pháp xây dựng tài sản dài hạn</v>
+        <v>Send Message</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>finance.sections.budgeting.title</v>
+        <v>contact.form.success</v>
       </c>
       <c r="B80" t="str">
-        <v>Smart Budgeting</v>
+        <v>Message sent successfully!</v>
       </c>
       <c r="C80" t="str">
-        <v>Quản Lý Chi Tiêu</v>
+        <v>Message sent successfully!</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>finance.sections.budgeting.description</v>
+        <v>contact.form.error</v>
       </c>
       <c r="B81" t="str">
-        <v>Practical tips for effective money management</v>
+        <v>Error sending message. Please try again.</v>
       </c>
       <c r="C81" t="str">
-        <v>Mẹo thực tế để quản lý tiền hiệu quả</v>
+        <v>Error sending message. Please try again.</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>finance.sections.planning.title</v>
+        <v>finance.title</v>
       </c>
       <c r="B82" t="str">
-        <v>Financial Planning</v>
+        <v>Personal Finance</v>
       </c>
       <c r="C82" t="str">
-        <v>Kế Hoạch Tài Chính</v>
+        <v>Quản Lý Tài Chính Cá Nhân</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>finance.sections.planning.description</v>
+        <v>finance.description</v>
       </c>
       <c r="B83" t="str">
-        <v>Setting and achieving financial goals</v>
+        <v>Insights and strategies for building financial independence</v>
       </c>
       <c r="C83" t="str">
-        <v>Thiết lập và đạt được mục tiêu tài chính</v>
+        <v>Những hiểu biết và chiến lược để xây dựng tự do tài chính</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>impact.title</v>
+        <v>finance.sections.investments.title</v>
       </c>
       <c r="B84" t="str">
-        <v>Social Impact</v>
+        <v>Investment Strategies</v>
       </c>
       <c r="C84" t="str">
-        <v>Tác Động Xã Hội</v>
+        <v>Chiến Lược Đầu Tư</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>impact.description</v>
+        <v>finance.sections.investments.description</v>
       </c>
       <c r="B85" t="str">
-        <v>Making a positive difference in the world</v>
+        <v>Long-term approaches to wealth building</v>
       </c>
       <c r="C85" t="str">
-        <v>Tạo ra những thay đổi tích cực cho thế giới</v>
+        <v>Phương pháp xây dựng tài sản dài hạn</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>impact.sections.projects.title</v>
+        <v>finance.sections.budgeting.title</v>
       </c>
       <c r="B86" t="str">
-        <v>Impact Projects</v>
+        <v>Smart Budgeting</v>
       </c>
       <c r="C86" t="str">
-        <v>Dự Án Tác Động</v>
+        <v>Quản Lý Chi Tiêu</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>impact.sections.projects.description</v>
+        <v>finance.sections.budgeting.description</v>
       </c>
       <c r="B87" t="str">
-        <v>Current initiatives and their outcomes</v>
+        <v>Practical tips for effective money management</v>
       </c>
       <c r="C87" t="str">
-        <v>Các sáng kiến hiện tại và kết quả</v>
+        <v>Mẹo thực tế để quản lý tiền hiệu quả</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>impact.sections.metrics.title</v>
+        <v>finance.sections.planning.title</v>
       </c>
       <c r="B88" t="str">
-        <v>Impact Metrics</v>
+        <v>Financial Planning</v>
       </c>
       <c r="C88" t="str">
-        <v>Đo Lường Tác Động</v>
+        <v>Kế Hoạch Tài Chính</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>impact.sections.metrics.description</v>
+        <v>finance.sections.planning.description</v>
       </c>
       <c r="B89" t="str">
-        <v>Measuring and tracking social impact</v>
+        <v>Setting and achieving financial goals</v>
       </c>
       <c r="C89" t="str">
-        <v>Đo lường và theo dõi tác động xã hội</v>
+        <v>Thiết lập và đạt được mục tiêu tài chính</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>impact.sections.collaboration.title</v>
+        <v>impact.title</v>
       </c>
       <c r="B90" t="str">
-        <v>Get Involved</v>
+        <v>Social Impact</v>
       </c>
       <c r="C90" t="str">
-        <v>Tham Gia</v>
+        <v>Tác Động Xã Hội</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>impact.sections.collaboration.description</v>
+        <v>impact.description</v>
       </c>
       <c r="B91" t="str">
-        <v>Ways to contribute and collaborate</v>
+        <v>Making a positive difference in the world</v>
       </c>
       <c r="C91" t="str">
-        <v>Cách đóng góp và hợp tác</v>
+        <v>Tạo ra những thay đổi tích cực cho thế giới</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>common.back_to_library</v>
+        <v>impact.sections.projects.title</v>
       </c>
       <c r="B92" t="str">
-        <v>Back to Library</v>
+        <v>Impact Projects</v>
       </c>
       <c r="C92" t="str">
-        <v>Quay Lại Thư Viện</v>
+        <v>Dự Án Tác Động</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
+        <v>impact.sections.projects.description</v>
+      </c>
+      <c r="B93" t="str">
+        <v>Current initiatives and their outcomes</v>
+      </c>
+      <c r="C93" t="str">
+        <v>Các sáng kiến hiện tại và kết quả</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>impact.sections.metrics.title</v>
+      </c>
+      <c r="B94" t="str">
+        <v>Impact Metrics</v>
+      </c>
+      <c r="C94" t="str">
+        <v>Đo Lường Tác Động</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>impact.sections.metrics.description</v>
+      </c>
+      <c r="B95" t="str">
+        <v>Measuring and tracking social impact</v>
+      </c>
+      <c r="C95" t="str">
+        <v>Đo lường và theo dõi tác động xã hội</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>impact.sections.collaboration.title</v>
+      </c>
+      <c r="B96" t="str">
+        <v>Get Involved</v>
+      </c>
+      <c r="C96" t="str">
+        <v>Tham Gia</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>impact.sections.collaboration.description</v>
+      </c>
+      <c r="B97" t="str">
+        <v>Ways to contribute and collaborate</v>
+      </c>
+      <c r="C97" t="str">
+        <v>Cách đóng góp và hợp tác</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>common.back_to_library</v>
+      </c>
+      <c r="B98" t="str">
+        <v>Back to Library</v>
+      </c>
+      <c r="C98" t="str">
+        <v>Quay Lại Thư Viện</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
         <v>common.published_on</v>
       </c>
-      <c r="B93" t="str">
+      <c r="B99" t="str">
         <v>Published on {{date}}</v>
       </c>
-      <c r="C93" t="str">
+      <c r="C99" t="str">
         <v>Xuất bản ngày {{date}}</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C93"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C99"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implement comprehensive translation system with localization support
</commit_message>
<xml_diff>
--- a/frontend/translations/translations.xlsx
+++ b/frontend/translations/translations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -915,590 +915,1063 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>resources.title</v>
+        <v>blog.metadata.separator</v>
       </c>
       <c r="B47" t="str">
-        <v>Resources</v>
+        <v>•</v>
       </c>
       <c r="C47" t="str">
-        <v>Tài Nguyên</v>
+        <v>•</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>resources.description</v>
+        <v>resources.title</v>
       </c>
       <c r="B48" t="str">
-        <v>A collection of tools, guides, and resources to help you on your journey</v>
+        <v>Resources</v>
       </c>
       <c r="C48" t="str">
-        <v>Bộ sưu tập công cụ, hướng dẫn và tài nguyên để hỗ trợ bạn trên hành trình của mình</v>
+        <v>Tài Nguyên</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>resources.tools</v>
+        <v>resources.description</v>
       </c>
       <c r="B49" t="str">
-        <v>Tools</v>
+        <v>A collection of tools, guides, and resources to help you on your journey</v>
       </c>
       <c r="C49" t="str">
-        <v>Công Cụ</v>
+        <v>Bộ sưu tập công cụ, hướng dẫn và tài nguyên để hỗ trợ bạn trên hành trình của mình</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>resources.guides</v>
+        <v>resources.tools</v>
       </c>
       <c r="B50" t="str">
-        <v>Guides</v>
+        <v>Tools</v>
       </c>
       <c r="C50" t="str">
-        <v>Hướng Dẫn</v>
+        <v>Công Cụ</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>about.title</v>
+        <v>resources.guides</v>
       </c>
       <c r="B51" t="str">
-        <v>About Me</v>
+        <v>Guides</v>
       </c>
       <c r="C51" t="str">
-        <v>Về Tôi</v>
+        <v>Hướng Dẫn</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>about.intro</v>
+        <v>about.title</v>
       </c>
       <c r="B52" t="str">
-        <v>Hi, I'm Jonathan. I'm passionate about technology and making a positive impact.</v>
+        <v>About Me</v>
       </c>
       <c r="C52" t="str">
-        <v>Xin chào, tôi là Jonathan. Tôi đam mê công nghệ và tạo ra những tác động tích cực.</v>
+        <v>Về Tôi</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>about.mission</v>
+        <v>about.intro</v>
       </c>
       <c r="B53" t="str">
-        <v>My mission is to help others leverage technology for positive change.</v>
+        <v>Hi, I'm Jonathan. I'm passionate about technology and making a positive impact.</v>
       </c>
       <c r="C53" t="str">
-        <v>Sứ mệnh của tôi là giúp mọi người tận dụng công nghệ để tạo ra những thay đổi tích cực.</v>
+        <v>Xin chào, tôi là Jonathan. Tôi đam mê công nghệ và tạo ra những tác động tích cực.</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>about.contact</v>
+        <v>about.mission</v>
       </c>
       <c r="B54" t="str">
-        <v>Get in Touch</v>
+        <v>My mission is to help others leverage technology for positive change.</v>
       </c>
       <c r="C54" t="str">
-        <v>Liên Hệ</v>
+        <v>Sứ mệnh của tôi là giúp mọi người tận dụng công nghệ để tạo ra những thay đổi tích cực.</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>about.background.title</v>
+        <v>about.contact</v>
       </c>
       <c r="B55" t="str">
-        <v>Background</v>
+        <v>Get in Touch</v>
       </c>
       <c r="C55" t="str">
-        <v>Giới Thiệu</v>
+        <v>Liên Hệ</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>about.background.content</v>
+        <v>about.background.title</v>
       </c>
       <c r="B56" t="str">
-        <v>As a Product Manager with a passion for technology and social impact, I bridge the gap between innovative solutions and human needs. My journey in product management has been driven by a commitment to creating meaningful digital experiences that make a difference.</v>
+        <v>Background</v>
       </c>
       <c r="C56" t="str">
-        <v>Là một Product Manager với niềm đam mê về công nghệ và tác động xã hội, tôi kết nối giữa các giải pháp sáng tạo và nhu cầu con người. Hành trình của tôi trong quản lý sản phẩm được thúc đẩy bởi cam kết tạo ra những trải nghiệm kỹ thuật số có ý nghĩa.</v>
+        <v>Giới Thiệu</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>about.expertise.title</v>
+        <v>about.background.content</v>
       </c>
       <c r="B57" t="str">
-        <v>Expertise</v>
+        <v>As a Product Manager with a passion for technology and social impact, I bridge the gap between innovative solutions and human needs. My journey in product management has been driven by a commitment to creating meaningful digital experiences that make a difference.</v>
       </c>
       <c r="C57" t="str">
-        <v>Chuyên Môn</v>
+        <v>Là một Product Manager với niềm đam mê về công nghệ và tác động xã hội, tôi kết nối giữa các giải pháp sáng tạo và nhu cầu con người. Hành trình của tôi trong quản lý sản phẩm được thúc đẩy bởi cam kết tạo ra những trải nghiệm kỹ thuật số có ý nghĩa.</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>about.expertise.skills.product_strategy</v>
+        <v>about.expertise.title</v>
       </c>
       <c r="B58" t="str">
-        <v>Product Strategy</v>
+        <v>Expertise</v>
       </c>
       <c r="C58" t="str">
-        <v>Chiến Lược Sản Phẩm</v>
+        <v>Chuyên Môn</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>about.expertise.skills.user_research</v>
+        <v>about.expertise.skills.product_strategy</v>
       </c>
       <c r="B59" t="str">
-        <v>User Research</v>
+        <v>Product Strategy</v>
       </c>
       <c r="C59" t="str">
-        <v>Nghiên Cứu Người Dùng</v>
+        <v>Chiến Lược Sản Phẩm</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>about.expertise.skills.agile</v>
+        <v>about.expertise.skills.user_research</v>
       </c>
       <c r="B60" t="str">
-        <v>Agile Management</v>
+        <v>User Research</v>
       </c>
       <c r="C60" t="str">
-        <v>Quản Lý Agile</v>
+        <v>Nghiên Cứu Người Dùng</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>about.expertise.skills.analytics</v>
+        <v>about.expertise.skills.agile</v>
       </c>
       <c r="B61" t="str">
-        <v>Data Analytics</v>
+        <v>Agile Management</v>
       </c>
       <c r="C61" t="str">
-        <v>Phân Tích Dữ Liệu</v>
+        <v>Quản Lý Agile</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>about.expertise.skills.technical</v>
+        <v>about.expertise.skills.analytics</v>
       </c>
       <c r="B62" t="str">
-        <v>Technical Leadership</v>
+        <v>Data Analytics</v>
       </c>
       <c r="C62" t="str">
-        <v>Lãnh Đạo Kỹ Thuật</v>
+        <v>Phân Tích Dữ Liệu</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>about.vision.title</v>
+        <v>about.expertise.skills.technical</v>
       </c>
       <c r="B63" t="str">
-        <v>Vision</v>
+        <v>Technical Leadership</v>
       </c>
       <c r="C63" t="str">
-        <v>Tầm Nhìn</v>
+        <v>Lãnh Đạo Kỹ Thuật</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>about.vision.content</v>
+        <v>about.vision.title</v>
       </c>
       <c r="B64" t="str">
-        <v>I believe in leveraging technology to create products that not only solve problems but also contribute positively to society. My goal is to lead product initiatives that combine innovation with social responsibility.</v>
+        <v>Vision</v>
       </c>
       <c r="C64" t="str">
-        <v>Tôi tin vào việc tận dụng công nghệ để tạo ra những sản phẩm không chỉ giải quyết vấn đề mà còn đóng góp tích cực cho xã hội. Mục tiêu của tôi là dẫn dắt các sáng kiến sản phẩm kết hợp đổi mới với trách nhiệm xã hội.</v>
+        <v>Tầm Nhìn</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>about.timeline.present.year</v>
+        <v>about.vision.content</v>
       </c>
       <c r="B65" t="str">
-        <v>2023 - Present</v>
+        <v>I believe in leveraging technology to create products that not only solve problems but also contribute positively to society. My goal is to lead product initiatives that combine innovation with social responsibility.</v>
       </c>
       <c r="C65" t="str">
-        <v>2023 - Hiện tại</v>
+        <v>Tôi tin vào việc tận dụng công nghệ để tạo ra những sản phẩm không chỉ giải quyết vấn đề mà còn đóng góp tích cực cho xã hội. Mục tiêu của tôi là dẫn dắt các sáng kiến sản phẩm kết hợp đổi mới với trách nhiệm xã hội.</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>about.timeline.present.title</v>
+        <v>about.timeline.present.year</v>
       </c>
       <c r="B66" t="str">
-        <v>Senior Product Manager</v>
+        <v>2023 - Present</v>
       </c>
       <c r="C66" t="str">
-        <v>Quản Lý Sản Phẩm Cao Cấp</v>
+        <v>2023 - Hiện tại</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>about.timeline.present.description</v>
+        <v>about.timeline.present.title</v>
       </c>
       <c r="B67" t="str">
-        <v>Leading innovative product initiatives</v>
+        <v>Senior Product Manager</v>
       </c>
       <c r="C67" t="str">
-        <v>Dẫn dắt các sáng kiến sản phẩm sáng tạo</v>
+        <v>Quản Lý Sản Phẩm Cao Cấp</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>about.timeline.past_1.year</v>
+        <v>about.timeline.present.description</v>
       </c>
       <c r="B68" t="str">
-        <v>2020 - 2023</v>
+        <v>Leading innovative product initiatives</v>
       </c>
       <c r="C68" t="str">
-        <v>2020 - 2023</v>
+        <v>Dẫn dắt các sáng kiến sản phẩm sáng tạo</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>about.timeline.past_1.title</v>
+        <v>about.timeline.past_1.year</v>
       </c>
       <c r="B69" t="str">
-        <v>Product Manager</v>
+        <v>2020 - 2023</v>
       </c>
       <c r="C69" t="str">
-        <v>Quản Lý Sản Phẩm</v>
+        <v>2020 - 2023</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>about.timeline.past_1.description</v>
+        <v>about.timeline.past_1.title</v>
       </c>
       <c r="B70" t="str">
-        <v>Driving user-centered product development</v>
+        <v>Product Manager</v>
       </c>
       <c r="C70" t="str">
-        <v>Thúc đẩy phát triển sản phẩm lấy người dùng làm trung tâm</v>
+        <v>Quản Lý Sản Phẩm</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>about.timeline.past_2.year</v>
+        <v>about.timeline.past_1.description</v>
       </c>
       <c r="B71" t="str">
-        <v>2018 - 2020</v>
+        <v>Driving user-centered product development</v>
       </c>
       <c r="C71" t="str">
-        <v>2018 - 2020</v>
+        <v>Thúc đẩy phát triển sản phẩm lấy người dùng làm trung tâm</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>about.timeline.past_2.title</v>
+        <v>about.timeline.past_2.year</v>
       </c>
       <c r="B72" t="str">
-        <v>Associate Product Manager</v>
+        <v>2018 - 2020</v>
       </c>
       <c r="C72" t="str">
-        <v>Quản Lý Sản Phẩm Phó</v>
+        <v>2018 - 2020</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>about.timeline.past_2.description</v>
+        <v>about.timeline.past_2.title</v>
       </c>
       <c r="B73" t="str">
-        <v>Building foundation in product management</v>
+        <v>Associate Product Manager</v>
       </c>
       <c r="C73" t="str">
-        <v>Xây dựng nền tảng trong quản lý sản phẩm</v>
+        <v>Quản Lý Sản Phẩm Phó</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>contact.title</v>
+        <v>about.timeline.past_2.description</v>
       </c>
       <c r="B74" t="str">
-        <v>Get in Touch</v>
+        <v>Building foundation in product management</v>
       </c>
       <c r="C74" t="str">
-        <v>Get in Touch</v>
+        <v>Xây dựng nền tảng trong quản lý sản phẩm</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>contact.description</v>
+        <v>contact.title</v>
       </c>
       <c r="B75" t="str">
-        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
+        <v>Get in Touch</v>
       </c>
       <c r="C75" t="str">
-        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
+        <v>Get in Touch</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>contact.form.name</v>
+        <v>contact.description</v>
       </c>
       <c r="B76" t="str">
-        <v>Your Name</v>
+        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
       </c>
       <c r="C76" t="str">
-        <v>Your Name</v>
+        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>contact.form.email</v>
+        <v>contact.form.name</v>
       </c>
       <c r="B77" t="str">
-        <v>Your Email</v>
+        <v>Your Name</v>
       </c>
       <c r="C77" t="str">
-        <v>Your Email</v>
+        <v>Your Name</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>contact.form.message</v>
+        <v>contact.form.email</v>
       </c>
       <c r="B78" t="str">
-        <v>Your Message</v>
+        <v>Your Email</v>
       </c>
       <c r="C78" t="str">
-        <v>Your Message</v>
+        <v>Your Email</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>contact.form.submit</v>
+        <v>contact.form.message</v>
       </c>
       <c r="B79" t="str">
-        <v>Send Message</v>
+        <v>Your Message</v>
       </c>
       <c r="C79" t="str">
-        <v>Send Message</v>
+        <v>Your Message</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>contact.form.success</v>
+        <v>contact.form.submit</v>
       </c>
       <c r="B80" t="str">
-        <v>Message sent successfully!</v>
+        <v>Send Message</v>
       </c>
       <c r="C80" t="str">
-        <v>Message sent successfully!</v>
+        <v>Send Message</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>contact.form.error</v>
+        <v>contact.form.success</v>
       </c>
       <c r="B81" t="str">
-        <v>Error sending message. Please try again.</v>
+        <v>Message sent successfully!</v>
       </c>
       <c r="C81" t="str">
-        <v>Error sending message. Please try again.</v>
+        <v>Message sent successfully!</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>finance.title</v>
+        <v>contact.form.error</v>
       </c>
       <c r="B82" t="str">
-        <v>Personal Finance</v>
+        <v>Error sending message. Please try again.</v>
       </c>
       <c r="C82" t="str">
-        <v>Quản Lý Tài Chính Cá Nhân</v>
+        <v>Error sending message. Please try again.</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>finance.description</v>
+        <v>finance.title</v>
       </c>
       <c r="B83" t="str">
-        <v>Insights and strategies for building financial independence</v>
+        <v>Personal Finance</v>
       </c>
       <c r="C83" t="str">
-        <v>Những hiểu biết và chiến lược để xây dựng tự do tài chính</v>
+        <v>Quản Lý Tài Chính Cá Nhân</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>finance.sections.investments.title</v>
+        <v>finance.description</v>
       </c>
       <c r="B84" t="str">
-        <v>Investment Strategies</v>
+        <v>Insights and strategies for building financial independence</v>
       </c>
       <c r="C84" t="str">
-        <v>Chiến Lược Đầu Tư</v>
+        <v>Những hiểu biết và chiến lược để xây dựng tự do tài chính</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>finance.sections.investments.description</v>
+        <v>finance.sections.investments.title</v>
       </c>
       <c r="B85" t="str">
-        <v>Long-term approaches to wealth building</v>
+        <v>Investment Strategies</v>
       </c>
       <c r="C85" t="str">
-        <v>Phương pháp xây dựng tài sản dài hạn</v>
+        <v>Chiến Lược Đầu Tư</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>finance.sections.budgeting.title</v>
+        <v>finance.sections.investments.description</v>
       </c>
       <c r="B86" t="str">
-        <v>Smart Budgeting</v>
+        <v>Long-term approaches to wealth building</v>
       </c>
       <c r="C86" t="str">
-        <v>Quản Lý Chi Tiêu</v>
+        <v>Phương pháp xây dựng tài sản dài hạn</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>finance.sections.budgeting.description</v>
+        <v>finance.sections.budgeting.title</v>
       </c>
       <c r="B87" t="str">
-        <v>Practical tips for effective money management</v>
+        <v>Smart Budgeting</v>
       </c>
       <c r="C87" t="str">
-        <v>Mẹo thực tế để quản lý tiền hiệu quả</v>
+        <v>Quản Lý Chi Tiêu</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>finance.sections.planning.title</v>
+        <v>finance.sections.budgeting.description</v>
       </c>
       <c r="B88" t="str">
-        <v>Financial Planning</v>
+        <v>Practical tips for effective money management</v>
       </c>
       <c r="C88" t="str">
-        <v>Kế Hoạch Tài Chính</v>
+        <v>Mẹo thực tế để quản lý tiền hiệu quả</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>finance.sections.planning.description</v>
+        <v>finance.sections.planning.title</v>
       </c>
       <c r="B89" t="str">
-        <v>Setting and achieving financial goals</v>
+        <v>Financial Planning</v>
       </c>
       <c r="C89" t="str">
-        <v>Thiết lập và đạt được mục tiêu tài chính</v>
+        <v>Kế Hoạch Tài Chính</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>impact.title</v>
+        <v>finance.sections.planning.description</v>
       </c>
       <c r="B90" t="str">
-        <v>Social Impact</v>
+        <v>Setting and achieving financial goals</v>
       </c>
       <c r="C90" t="str">
-        <v>Tác Động Xã Hội</v>
+        <v>Thiết lập và đạt được mục tiêu tài chính</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>impact.description</v>
+        <v>impact.title</v>
       </c>
       <c r="B91" t="str">
-        <v>Making a positive difference in the world</v>
+        <v>Social Impact</v>
       </c>
       <c r="C91" t="str">
-        <v>Tạo ra những thay đổi tích cực cho thế giới</v>
+        <v>Tác Động Xã Hội</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>impact.sections.projects.title</v>
+        <v>impact.description</v>
       </c>
       <c r="B92" t="str">
-        <v>Impact Projects</v>
+        <v>Making a positive difference in the world</v>
       </c>
       <c r="C92" t="str">
-        <v>Dự Án Tác Động</v>
+        <v>Tạo ra những thay đổi tích cực cho thế giới</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>impact.sections.projects.description</v>
+        <v>impact.sections.projects.title</v>
       </c>
       <c r="B93" t="str">
-        <v>Current initiatives and their outcomes</v>
+        <v>Impact Projects</v>
       </c>
       <c r="C93" t="str">
-        <v>Các sáng kiến hiện tại và kết quả</v>
+        <v>Dự Án Tác Động</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>impact.sections.metrics.title</v>
+        <v>impact.sections.projects.description</v>
       </c>
       <c r="B94" t="str">
-        <v>Impact Metrics</v>
+        <v>Current initiatives and their outcomes</v>
       </c>
       <c r="C94" t="str">
-        <v>Đo Lường Tác Động</v>
+        <v>Các sáng kiến hiện tại và kết quả</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>impact.sections.metrics.description</v>
+        <v>impact.sections.metrics.title</v>
       </c>
       <c r="B95" t="str">
-        <v>Measuring and tracking social impact</v>
+        <v>Impact Metrics</v>
       </c>
       <c r="C95" t="str">
-        <v>Đo lường và theo dõi tác động xã hội</v>
+        <v>Đo Lường Tác Động</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>impact.sections.collaboration.title</v>
+        <v>impact.sections.metrics.description</v>
       </c>
       <c r="B96" t="str">
-        <v>Get Involved</v>
+        <v>Measuring and tracking social impact</v>
       </c>
       <c r="C96" t="str">
-        <v>Tham Gia</v>
+        <v>Đo lường và theo dõi tác động xã hội</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>impact.sections.collaboration.description</v>
+        <v>impact.sections.collaboration.title</v>
       </c>
       <c r="B97" t="str">
-        <v>Ways to contribute and collaborate</v>
+        <v>Get Involved</v>
       </c>
       <c r="C97" t="str">
-        <v>Cách đóng góp và hợp tác</v>
+        <v>Tham Gia</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>common.back_to_library</v>
+        <v>impact.sections.collaboration.description</v>
       </c>
       <c r="B98" t="str">
-        <v>Back to Library</v>
+        <v>Ways to contribute and collaborate</v>
       </c>
       <c r="C98" t="str">
-        <v>Quay Lại Thư Viện</v>
+        <v>Cách đóng góp và hợp tác</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
+        <v>common.back_to_library</v>
+      </c>
+      <c r="B99" t="str">
+        <v>Back to Library</v>
+      </c>
+      <c r="C99" t="str">
+        <v>Quay Lại Thư Viện</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
         <v>common.published_on</v>
       </c>
-      <c r="B99" t="str">
+      <c r="B100" t="str">
         <v>Published on {{date}}</v>
       </c>
-      <c r="C99" t="str">
+      <c r="C100" t="str">
         <v>Xuất bản ngày {{date}}</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>common.explore</v>
+      </c>
+      <c r="B101" t="str">
+        <v>Explore Section</v>
+      </c>
+      <c r="C101" t="str">
+        <v>Khám Phá</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>auth.login.title</v>
+      </c>
+      <c r="B102" t="str">
+        <v>Sign in to your account</v>
+      </c>
+      <c r="C102" t="str">
+        <v>Đăng nhập vào tài khoản của bạn</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>auth.login.email_label</v>
+      </c>
+      <c r="B103" t="str">
+        <v>Email address</v>
+      </c>
+      <c r="C103" t="str">
+        <v>Địa chỉ email</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>auth.login.email_placeholder</v>
+      </c>
+      <c r="B104" t="str">
+        <v>Email address</v>
+      </c>
+      <c r="C104" t="str">
+        <v>Địa chỉ email</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>auth.login.password_label</v>
+      </c>
+      <c r="B105" t="str">
+        <v>Password</v>
+      </c>
+      <c r="C105" t="str">
+        <v>Mật khẩu</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>auth.login.password_placeholder</v>
+      </c>
+      <c r="B106" t="str">
+        <v>Password</v>
+      </c>
+      <c r="C106" t="str">
+        <v>Mật khẩu</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>auth.login.forgot_password</v>
+      </c>
+      <c r="B107" t="str">
+        <v>Forgot your password?</v>
+      </c>
+      <c r="C107" t="str">
+        <v>Quên mật khẩu?</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>auth.login.submit_button</v>
+      </c>
+      <c r="B108" t="str">
+        <v>Sign in</v>
+      </c>
+      <c r="C108" t="str">
+        <v>Đăng nhập</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>auth.login.submitting</v>
+      </c>
+      <c r="B109" t="str">
+        <v>Signing in...</v>
+      </c>
+      <c r="C109" t="str">
+        <v>Đang đăng nhập...</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>auth.login.need_account</v>
+      </c>
+      <c r="B110" t="str">
+        <v>Need an account?</v>
+      </c>
+      <c r="C110" t="str">
+        <v>Chưa có tài khoản?</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>auth.login.sign_up_link</v>
+      </c>
+      <c r="B111" t="str">
+        <v>Sign up</v>
+      </c>
+      <c r="C111" t="str">
+        <v>Đăng ký</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>auth.login.error</v>
+      </c>
+      <c r="B112" t="str">
+        <v>Failed to log in: {{message}}</v>
+      </c>
+      <c r="C112" t="str">
+        <v>Đăng nhập thất bại: {{message}}</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>auth.signup.title</v>
+      </c>
+      <c r="B113" t="str">
+        <v>Create your account</v>
+      </c>
+      <c r="C113" t="str">
+        <v>Tạo tài khoản của bạn</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>auth.signup.email_label</v>
+      </c>
+      <c r="B114" t="str">
+        <v>Email address</v>
+      </c>
+      <c r="C114" t="str">
+        <v>Địa chỉ email</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>auth.signup.email_placeholder</v>
+      </c>
+      <c r="B115" t="str">
+        <v>Email address</v>
+      </c>
+      <c r="C115" t="str">
+        <v>Địa chỉ email</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>auth.signup.password_label</v>
+      </c>
+      <c r="B116" t="str">
+        <v>Password</v>
+      </c>
+      <c r="C116" t="str">
+        <v>Mật khẩu</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>auth.signup.password_placeholder</v>
+      </c>
+      <c r="B117" t="str">
+        <v>Password</v>
+      </c>
+      <c r="C117" t="str">
+        <v>Mật khẩu</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>auth.signup.confirm_password_label</v>
+      </c>
+      <c r="B118" t="str">
+        <v>Confirm Password</v>
+      </c>
+      <c r="C118" t="str">
+        <v>Xác nhận mật khẩu</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>auth.signup.confirm_password_placeholder</v>
+      </c>
+      <c r="B119" t="str">
+        <v>Confirm Password</v>
+      </c>
+      <c r="C119" t="str">
+        <v>Xác nhận mật khẩu</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>auth.signup.submit_button</v>
+      </c>
+      <c r="B120" t="str">
+        <v>Sign up</v>
+      </c>
+      <c r="C120" t="str">
+        <v>Đăng ký</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>auth.signup.submitting</v>
+      </c>
+      <c r="B121" t="str">
+        <v>Creating account...</v>
+      </c>
+      <c r="C121" t="str">
+        <v>Đang tạo tài khoản...</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>auth.signup.have_account</v>
+      </c>
+      <c r="B122" t="str">
+        <v>Already have an account?</v>
+      </c>
+      <c r="C122" t="str">
+        <v>Đã có tài khoản?</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>auth.signup.login_link</v>
+      </c>
+      <c r="B123" t="str">
+        <v>Log in</v>
+      </c>
+      <c r="C123" t="str">
+        <v>Đăng nhập</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>auth.signup.error</v>
+      </c>
+      <c r="B124" t="str">
+        <v>Failed to create an account: {{message}}</v>
+      </c>
+      <c r="C124" t="str">
+        <v>Tạo tài khoản thất bại: {{message}}</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>auth.signup.passwords_not_match</v>
+      </c>
+      <c r="B125" t="str">
+        <v>Passwords do not match</v>
+      </c>
+      <c r="C125" t="str">
+        <v>Mật khẩu không khớp</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>auth.forgot_password.title</v>
+      </c>
+      <c r="B126" t="str">
+        <v>Reset your password</v>
+      </c>
+      <c r="C126" t="str">
+        <v>Đặt lại mật khẩu của bạn</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>auth.forgot_password.email_label</v>
+      </c>
+      <c r="B127" t="str">
+        <v>Email address</v>
+      </c>
+      <c r="C127" t="str">
+        <v>Địa chỉ email</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>auth.forgot_password.email_placeholder</v>
+      </c>
+      <c r="B128" t="str">
+        <v>Email address</v>
+      </c>
+      <c r="C128" t="str">
+        <v>Địa chỉ email</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>auth.forgot_password.submit_button</v>
+      </c>
+      <c r="B129" t="str">
+        <v>Reset Password</v>
+      </c>
+      <c r="C129" t="str">
+        <v>Đặt lại mật khẩu</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>auth.forgot_password.submitting</v>
+      </c>
+      <c r="B130" t="str">
+        <v>Processing...</v>
+      </c>
+      <c r="C130" t="str">
+        <v>Đang xử lý...</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>auth.forgot_password.back_to_login</v>
+      </c>
+      <c r="B131" t="str">
+        <v>Back to login</v>
+      </c>
+      <c r="C131" t="str">
+        <v>Quay lại đăng nhập</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>auth.forgot_password.error</v>
+      </c>
+      <c r="B132" t="str">
+        <v>Failed to reset password: {{message}}</v>
+      </c>
+      <c r="C132" t="str">
+        <v>Đặt lại mật khẩu thất bại: {{message}}</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>auth.forgot_password.success_message</v>
+      </c>
+      <c r="B133" t="str">
+        <v>Check your inbox for further instructions</v>
+      </c>
+      <c r="C133" t="str">
+        <v>Kiểm tra hộp thư của bạn để biết hướng dẫn tiếp theo</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>auth.profile.title</v>
+      </c>
+      <c r="B134" t="str">
+        <v>Profile</v>
+      </c>
+      <c r="C134" t="str">
+        <v>Hồ sơ</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>auth.profile.user_info_title</v>
+      </c>
+      <c r="B135" t="str">
+        <v>User Information</v>
+      </c>
+      <c r="C135" t="str">
+        <v>Thông tin người dùng</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>auth.profile.user_info_description</v>
+      </c>
+      <c r="B136" t="str">
+        <v>Personal details and account settings.</v>
+      </c>
+      <c r="C136" t="str">
+        <v>Thông tin cá nhân và cài đặt tài khoản.</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>auth.profile.email_label</v>
+      </c>
+      <c r="B137" t="str">
+        <v>Email</v>
+      </c>
+      <c r="C137" t="str">
+        <v>Email</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>auth.profile.email_verified_label</v>
+      </c>
+      <c r="B138" t="str">
+        <v>Email verified</v>
+      </c>
+      <c r="C138" t="str">
+        <v>Email đã xác minh</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>auth.profile.yes</v>
+      </c>
+      <c r="B139" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="C139" t="str">
+        <v>Có</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>auth.profile.no</v>
+      </c>
+      <c r="B140" t="str">
+        <v>No</v>
+      </c>
+      <c r="C140" t="str">
+        <v>Không</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>auth.profile.logout_button</v>
+      </c>
+      <c r="B141" t="str">
+        <v>Log Out</v>
+      </c>
+      <c r="C141" t="str">
+        <v>Đăng xuất</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>auth.profile.error</v>
+      </c>
+      <c r="B142" t="str">
+        <v>Failed to log out</v>
+      </c>
+      <c r="C142" t="str">
+        <v>Đăng xuất thất bại</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C99"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C142"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add profile navigation label to English and Vietnamese translations
</commit_message>
<xml_diff>
--- a/frontend/translations/translations.xlsx
+++ b/frontend/translations/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanvu/Library/Mobile Documents/com~apple~CloudDocs/Documents/Knowledge Hub/AI/Code/ht-catalyst/frontend/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695E8282-10B5-2745-B5F0-89FDA271E058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17196BDE-A036-5649-A8E9-BBAE50A22560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="387">
   <si>
     <t>key</t>
   </si>
@@ -1172,6 +1172,15 @@
   </si>
   <si>
     <t>nav.signup</t>
+  </si>
+  <si>
+    <t>nav.profile</t>
+  </si>
+  <si>
+    <t>Tài khoản của bạn</t>
+  </si>
+  <si>
+    <t>Thư viện</t>
   </si>
 </sst>
 </file>
@@ -1548,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C145"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1612,7 +1621,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1694,1041 +1703,1041 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>384</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>355</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C42" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
-        <v>123</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C49" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C50" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C51" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B52" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C52" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C54" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B56" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C56" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B57" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C57" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C59" t="s">
-        <v>17</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B60" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C60" t="s">
-        <v>160</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B61" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C61" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B62" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C62" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B63" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C63" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B64" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C64" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B65" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C65" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B66" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C66" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B67" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C67" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B68" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C68" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B69" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C69" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B70" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C70" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B71" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C71" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B72" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C72" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B73" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C73" t="s">
-        <v>118</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B74" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C74" t="s">
-        <v>200</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B75" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C75" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B76" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C76" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B77" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C77" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>207</v>
       </c>
       <c r="C78" t="s">
-        <v>154</v>
+        <v>208</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B79" t="s">
-        <v>211</v>
+        <v>154</v>
       </c>
       <c r="C79" t="s">
-        <v>211</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B80" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C80" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B81" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C81" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B82" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C82" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B83" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C83" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B84" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C84" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B85" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C85" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B86" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C86" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B87" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C87" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B88" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C88" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B89" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C89" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B90" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C90" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B91" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C91" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B92" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C92" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B93" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C93" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B94" t="s">
-        <v>120</v>
+        <v>246</v>
       </c>
       <c r="C94" t="s">
-        <v>23</v>
+        <v>247</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B95" t="s">
-        <v>250</v>
+        <v>120</v>
       </c>
       <c r="C95" t="s">
-        <v>251</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C96" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B97" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C97" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B98" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C98" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B99" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C99" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B100" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C100" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B101" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C101" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B102" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C102" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B103" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C103" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B104" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C104" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B105" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C105" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B106" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C106" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B107" t="s">
         <v>283</v>
@@ -2739,18 +2748,18 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B108" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C108" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B109" t="s">
         <v>287</v>
@@ -2761,95 +2770,95 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B110" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C110" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B111" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C111" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B112" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C112" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B113" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C113" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B114" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C114" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B115" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C115" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B116" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C116" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B117" t="s">
-        <v>283</v>
+        <v>309</v>
       </c>
       <c r="C117" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B118" t="s">
         <v>283</v>
@@ -2860,18 +2869,18 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B119" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C119" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B120" t="s">
         <v>287</v>
@@ -2882,18 +2891,18 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B121" t="s">
-        <v>316</v>
+        <v>287</v>
       </c>
       <c r="C121" t="s">
-        <v>317</v>
+        <v>288</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B122" t="s">
         <v>316</v>
@@ -2904,95 +2913,95 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B123" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="C123" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B124" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="C124" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B125" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C125" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B126" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C126" t="s">
-        <v>295</v>
+        <v>325</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B127" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C127" t="s">
-        <v>330</v>
+        <v>295</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B128" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C128" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B129" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C129" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B130" t="s">
-        <v>283</v>
+        <v>335</v>
       </c>
       <c r="C130" t="s">
-        <v>284</v>
+        <v>336</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B131" t="s">
         <v>283</v>
@@ -3003,162 +3012,173 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B132" t="s">
-        <v>340</v>
+        <v>283</v>
       </c>
       <c r="C132" t="s">
-        <v>341</v>
+        <v>284</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B133" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C133" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B134" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C134" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B135" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C135" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B136" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C136" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B137" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C137" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B138" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C138" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B139" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C139" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B140" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C140" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B141" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C141" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B142" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C142" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B143" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C143" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B144" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C144" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>374</v>
+      </c>
+      <c r="B145" t="s">
+        <v>375</v>
+      </c>
+      <c r="C145" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
         <v>377</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B146" t="s">
         <v>378</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C146" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A13:C145 A1:C8" numberStoredAsText="1"/>
+    <ignoredError sqref="A14:C146 A1:C4 A6:C8 A5:B5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add AI in Product Development blog post and update related components
</commit_message>
<xml_diff>
--- a/frontend/translations/translations.xlsx
+++ b/frontend/translations/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanvu/Library/Mobile Documents/com~apple~CloudDocs/Documents/Knowledge Hub/AI/Code/ht-catalyst/frontend/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17196BDE-A036-5649-A8E9-BBAE50A22560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBD5A88-75BA-4D46-B69E-5A56A01EAB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
     <t>site.title</t>
   </si>
   <si>
-    <t>PM Jonathan</t>
-  </si>
-  <si>
     <t>site.description</t>
   </si>
   <si>
@@ -1181,6 +1178,9 @@
   </si>
   <si>
     <t>Thư viện</t>
+  </si>
+  <si>
+    <t>KienNotes.AI</t>
   </si>
 </sst>
 </file>
@@ -1560,7 +1560,7 @@
   <dimension ref="A1:C146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1585,1600 +1585,1600 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>386</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>379</v>
+      </c>
+      <c r="B10" t="s">
         <v>380</v>
       </c>
-      <c r="B10" t="s">
-        <v>381</v>
-      </c>
       <c r="C10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B11" t="s">
+        <v>302</v>
+      </c>
+      <c r="C11" t="s">
         <v>303</v>
-      </c>
-      <c r="C11" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B12" t="s">
+        <v>374</v>
+      </c>
+      <c r="C12" t="s">
         <v>375</v>
-      </c>
-      <c r="C12" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>383</v>
+      </c>
+      <c r="B13" t="s">
+        <v>354</v>
+      </c>
+      <c r="C13" t="s">
         <v>384</v>
-      </c>
-      <c r="B13" t="s">
-        <v>355</v>
-      </c>
-      <c r="C13" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
         <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>41</v>
-      </c>
-      <c r="C20" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
         <v>49</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>50</v>
-      </c>
-      <c r="C23" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
         <v>52</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>53</v>
-      </c>
-      <c r="C24" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>56</v>
-      </c>
-      <c r="C25" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
         <v>58</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>59</v>
-      </c>
-      <c r="C26" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
         <v>61</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>62</v>
-      </c>
-      <c r="C27" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
         <v>64</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>65</v>
-      </c>
-      <c r="C28" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
         <v>67</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>68</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
         <v>70</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>71</v>
-      </c>
-      <c r="C30" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
         <v>73</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>74</v>
-      </c>
-      <c r="C31" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="s">
         <v>76</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>77</v>
-      </c>
-      <c r="C32" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" t="s">
         <v>79</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>80</v>
-      </c>
-      <c r="C33" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" t="s">
         <v>82</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>83</v>
-      </c>
-      <c r="C34" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
         <v>85</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>86</v>
-      </c>
-      <c r="C35" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" t="s">
         <v>88</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>89</v>
-      </c>
-      <c r="C36" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" t="s">
         <v>91</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>92</v>
-      </c>
-      <c r="C37" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" t="s">
         <v>94</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>95</v>
-      </c>
-      <c r="C38" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" t="s">
         <v>98</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>99</v>
-      </c>
-      <c r="C40" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" t="s">
         <v>101</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>102</v>
-      </c>
-      <c r="C41" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" t="s">
         <v>104</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>105</v>
-      </c>
-      <c r="C42" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" t="s">
         <v>107</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>108</v>
-      </c>
-      <c r="C43" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
         <v>110</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>111</v>
-      </c>
-      <c r="C44" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" t="s">
         <v>113</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>114</v>
-      </c>
-      <c r="C45" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" t="s">
         <v>116</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>117</v>
-      </c>
-      <c r="C46" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" t="s">
         <v>119</v>
       </c>
-      <c r="B47" t="s">
-        <v>120</v>
-      </c>
       <c r="C47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" t="s">
         <v>121</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>122</v>
-      </c>
-      <c r="C48" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" t="s">
         <v>124</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>125</v>
-      </c>
-      <c r="C49" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B50" t="s">
         <v>127</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>128</v>
-      </c>
-      <c r="C50" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" t="s">
         <v>130</v>
       </c>
-      <c r="B51" t="s">
-        <v>131</v>
-      </c>
       <c r="C51" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" t="s">
         <v>132</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>133</v>
-      </c>
-      <c r="C52" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>134</v>
+      </c>
+      <c r="B53" t="s">
         <v>135</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>136</v>
-      </c>
-      <c r="C53" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" t="s">
         <v>138</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>139</v>
-      </c>
-      <c r="C54" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>140</v>
+      </c>
+      <c r="B55" t="s">
         <v>141</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>142</v>
-      </c>
-      <c r="C55" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" t="s">
         <v>144</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>145</v>
-      </c>
-      <c r="C56" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>146</v>
+      </c>
+      <c r="B57" t="s">
         <v>147</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>148</v>
-      </c>
-      <c r="C57" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>149</v>
+      </c>
+      <c r="B58" t="s">
         <v>150</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>151</v>
-      </c>
-      <c r="C58" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59" t="s">
         <v>153</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>154</v>
-      </c>
-      <c r="C59" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" t="s">
         <v>156</v>
       </c>
-      <c r="B60" t="s">
-        <v>157</v>
-      </c>
       <c r="C60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" t="s">
         <v>158</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>159</v>
-      </c>
-      <c r="C61" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" t="s">
         <v>161</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>162</v>
-      </c>
-      <c r="C62" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>163</v>
+      </c>
+      <c r="B63" t="s">
         <v>164</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>165</v>
-      </c>
-      <c r="C63" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>166</v>
+      </c>
+      <c r="B64" t="s">
         <v>167</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>168</v>
-      </c>
-      <c r="C64" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>169</v>
+      </c>
+      <c r="B65" t="s">
         <v>170</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>171</v>
-      </c>
-      <c r="C65" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>172</v>
+      </c>
+      <c r="B66" t="s">
         <v>173</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>174</v>
-      </c>
-      <c r="C66" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>175</v>
+      </c>
+      <c r="B67" t="s">
         <v>176</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>177</v>
-      </c>
-      <c r="C67" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>178</v>
+      </c>
+      <c r="B68" t="s">
         <v>179</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>180</v>
-      </c>
-      <c r="C68" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" t="s">
         <v>182</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>183</v>
-      </c>
-      <c r="C69" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>184</v>
+      </c>
+      <c r="B70" t="s">
         <v>185</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>186</v>
-      </c>
-      <c r="C70" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>187</v>
+      </c>
+      <c r="B71" t="s">
         <v>188</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>189</v>
-      </c>
-      <c r="C71" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>190</v>
+      </c>
+      <c r="B72" t="s">
         <v>191</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>192</v>
-      </c>
-      <c r="C72" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>193</v>
+      </c>
+      <c r="B73" t="s">
         <v>194</v>
       </c>
-      <c r="B73" t="s">
-        <v>195</v>
-      </c>
       <c r="C73" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>195</v>
+      </c>
+      <c r="B74" t="s">
         <v>196</v>
       </c>
-      <c r="B74" t="s">
-        <v>197</v>
-      </c>
       <c r="C74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>197</v>
+      </c>
+      <c r="B75" t="s">
         <v>198</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>199</v>
-      </c>
-      <c r="C75" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>200</v>
+      </c>
+      <c r="B76" t="s">
         <v>201</v>
       </c>
-      <c r="B76" t="s">
-        <v>202</v>
-      </c>
       <c r="C76" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>202</v>
+      </c>
+      <c r="B77" t="s">
         <v>203</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>204</v>
-      </c>
-      <c r="C77" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>205</v>
+      </c>
+      <c r="B78" t="s">
         <v>206</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>207</v>
-      </c>
-      <c r="C78" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>209</v>
+      </c>
+      <c r="B80" t="s">
         <v>210</v>
       </c>
-      <c r="B80" t="s">
-        <v>211</v>
-      </c>
       <c r="C80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>211</v>
+      </c>
+      <c r="B81" t="s">
         <v>212</v>
       </c>
-      <c r="B81" t="s">
-        <v>213</v>
-      </c>
       <c r="C81" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>213</v>
+      </c>
+      <c r="B82" t="s">
         <v>214</v>
       </c>
-      <c r="B82" t="s">
-        <v>215</v>
-      </c>
       <c r="C82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>215</v>
+      </c>
+      <c r="B83" t="s">
         <v>216</v>
       </c>
-      <c r="B83" t="s">
-        <v>217</v>
-      </c>
       <c r="C83" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>217</v>
+      </c>
+      <c r="B84" t="s">
         <v>218</v>
       </c>
-      <c r="B84" t="s">
-        <v>219</v>
-      </c>
       <c r="C84" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>219</v>
+      </c>
+      <c r="B85" t="s">
         <v>220</v>
       </c>
-      <c r="B85" t="s">
-        <v>221</v>
-      </c>
       <c r="C85" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>221</v>
+      </c>
+      <c r="B86" t="s">
         <v>222</v>
       </c>
-      <c r="B86" t="s">
-        <v>223</v>
-      </c>
       <c r="C86" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>223</v>
+      </c>
+      <c r="B87" t="s">
         <v>224</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>225</v>
-      </c>
-      <c r="C87" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>226</v>
+      </c>
+      <c r="B88" t="s">
         <v>227</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>228</v>
-      </c>
-      <c r="C88" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>229</v>
+      </c>
+      <c r="B89" t="s">
         <v>230</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>231</v>
-      </c>
-      <c r="C89" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>232</v>
+      </c>
+      <c r="B90" t="s">
         <v>233</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>234</v>
-      </c>
-      <c r="C90" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>235</v>
+      </c>
+      <c r="B91" t="s">
         <v>236</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>237</v>
-      </c>
-      <c r="C91" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>238</v>
+      </c>
+      <c r="B92" t="s">
         <v>239</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>240</v>
-      </c>
-      <c r="C92" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>241</v>
+      </c>
+      <c r="B93" t="s">
         <v>242</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>243</v>
-      </c>
-      <c r="C93" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>244</v>
+      </c>
+      <c r="B94" t="s">
         <v>245</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>246</v>
-      </c>
-      <c r="C94" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B95" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C95" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>248</v>
+      </c>
+      <c r="B96" t="s">
         <v>249</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>250</v>
-      </c>
-      <c r="C96" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>251</v>
+      </c>
+      <c r="B97" t="s">
         <v>252</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>253</v>
-      </c>
-      <c r="C97" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>254</v>
+      </c>
+      <c r="B98" t="s">
         <v>255</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>256</v>
-      </c>
-      <c r="C98" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>257</v>
+      </c>
+      <c r="B99" t="s">
         <v>258</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>259</v>
-      </c>
-      <c r="C99" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>260</v>
+      </c>
+      <c r="B100" t="s">
         <v>261</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>262</v>
-      </c>
-      <c r="C100" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>263</v>
+      </c>
+      <c r="B101" t="s">
         <v>264</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>265</v>
-      </c>
-      <c r="C101" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>266</v>
+      </c>
+      <c r="B102" t="s">
         <v>267</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>268</v>
-      </c>
-      <c r="C102" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>269</v>
+      </c>
+      <c r="B103" t="s">
         <v>270</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>271</v>
-      </c>
-      <c r="C103" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>272</v>
+      </c>
+      <c r="B104" t="s">
         <v>273</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>274</v>
-      </c>
-      <c r="C104" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>275</v>
+      </c>
+      <c r="B105" t="s">
         <v>276</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>277</v>
-      </c>
-      <c r="C105" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>278</v>
+      </c>
+      <c r="B106" t="s">
         <v>279</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>280</v>
-      </c>
-      <c r="C106" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>281</v>
+      </c>
+      <c r="B107" t="s">
         <v>282</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>283</v>
-      </c>
-      <c r="C107" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B108" t="s">
+        <v>282</v>
+      </c>
+      <c r="C108" t="s">
         <v>283</v>
-      </c>
-      <c r="C108" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>285</v>
+      </c>
+      <c r="B109" t="s">
         <v>286</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>287</v>
-      </c>
-      <c r="C109" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B110" t="s">
+        <v>286</v>
+      </c>
+      <c r="C110" t="s">
         <v>287</v>
-      </c>
-      <c r="C110" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>289</v>
+      </c>
+      <c r="B111" t="s">
         <v>290</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>291</v>
-      </c>
-      <c r="C111" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>292</v>
+      </c>
+      <c r="B112" t="s">
         <v>293</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>294</v>
-      </c>
-      <c r="C112" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>295</v>
+      </c>
+      <c r="B113" t="s">
         <v>296</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>297</v>
-      </c>
-      <c r="C113" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>298</v>
+      </c>
+      <c r="B114" t="s">
         <v>299</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>300</v>
-      </c>
-      <c r="C114" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>301</v>
+      </c>
+      <c r="B115" t="s">
         <v>302</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>303</v>
-      </c>
-      <c r="C115" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>304</v>
+      </c>
+      <c r="B116" t="s">
         <v>305</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>306</v>
-      </c>
-      <c r="C116" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>307</v>
+      </c>
+      <c r="B117" t="s">
         <v>308</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>309</v>
-      </c>
-      <c r="C117" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B118" t="s">
+        <v>282</v>
+      </c>
+      <c r="C118" t="s">
         <v>283</v>
-      </c>
-      <c r="C118" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B119" t="s">
+        <v>282</v>
+      </c>
+      <c r="C119" t="s">
         <v>283</v>
-      </c>
-      <c r="C119" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B120" t="s">
+        <v>286</v>
+      </c>
+      <c r="C120" t="s">
         <v>287</v>
-      </c>
-      <c r="C120" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B121" t="s">
+        <v>286</v>
+      </c>
+      <c r="C121" t="s">
         <v>287</v>
-      </c>
-      <c r="C121" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>314</v>
+      </c>
+      <c r="B122" t="s">
         <v>315</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>316</v>
-      </c>
-      <c r="C122" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B123" t="s">
+        <v>315</v>
+      </c>
+      <c r="C123" t="s">
         <v>316</v>
-      </c>
-      <c r="C123" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B124" t="s">
+        <v>302</v>
+      </c>
+      <c r="C124" t="s">
         <v>303</v>
-      </c>
-      <c r="C124" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>319</v>
+      </c>
+      <c r="B125" t="s">
         <v>320</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>321</v>
-      </c>
-      <c r="C125" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>322</v>
+      </c>
+      <c r="B126" t="s">
         <v>323</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>324</v>
-      </c>
-      <c r="C126" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>325</v>
+      </c>
+      <c r="B127" t="s">
         <v>326</v>
       </c>
-      <c r="B127" t="s">
-        <v>327</v>
-      </c>
       <c r="C127" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>327</v>
+      </c>
+      <c r="B128" t="s">
         <v>328</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
         <v>329</v>
-      </c>
-      <c r="C128" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>330</v>
+      </c>
+      <c r="B129" t="s">
         <v>331</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" t="s">
         <v>332</v>
-      </c>
-      <c r="C129" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>333</v>
+      </c>
+      <c r="B130" t="s">
         <v>334</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" t="s">
         <v>335</v>
-      </c>
-      <c r="C130" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B131" t="s">
+        <v>282</v>
+      </c>
+      <c r="C131" t="s">
         <v>283</v>
-      </c>
-      <c r="C131" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B132" t="s">
+        <v>282</v>
+      </c>
+      <c r="C132" t="s">
         <v>283</v>
-      </c>
-      <c r="C132" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>338</v>
+      </c>
+      <c r="B133" t="s">
         <v>339</v>
       </c>
-      <c r="B133" t="s">
+      <c r="C133" t="s">
         <v>340</v>
-      </c>
-      <c r="C133" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>341</v>
+      </c>
+      <c r="B134" t="s">
         <v>342</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>343</v>
-      </c>
-      <c r="C134" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>344</v>
+      </c>
+      <c r="B135" t="s">
         <v>345</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>346</v>
-      </c>
-      <c r="C135" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>347</v>
+      </c>
+      <c r="B136" t="s">
         <v>348</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C136" t="s">
         <v>349</v>
-      </c>
-      <c r="C136" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>350</v>
+      </c>
+      <c r="B137" t="s">
         <v>351</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C137" t="s">
         <v>352</v>
-      </c>
-      <c r="C137" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>353</v>
+      </c>
+      <c r="B138" t="s">
         <v>354</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
         <v>355</v>
-      </c>
-      <c r="C138" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>356</v>
+      </c>
+      <c r="B139" t="s">
         <v>357</v>
       </c>
-      <c r="B139" t="s">
+      <c r="C139" t="s">
         <v>358</v>
-      </c>
-      <c r="C139" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>359</v>
+      </c>
+      <c r="B140" t="s">
         <v>360</v>
       </c>
-      <c r="B140" t="s">
+      <c r="C140" t="s">
         <v>361</v>
-      </c>
-      <c r="C140" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>362</v>
+      </c>
+      <c r="B141" t="s">
         <v>363</v>
       </c>
-      <c r="B141" t="s">
-        <v>364</v>
-      </c>
       <c r="C141" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>364</v>
+      </c>
+      <c r="B142" t="s">
         <v>365</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C142" t="s">
         <v>366</v>
-      </c>
-      <c r="C142" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
+        <v>367</v>
+      </c>
+      <c r="B143" t="s">
         <v>368</v>
       </c>
-      <c r="B143" t="s">
+      <c r="C143" t="s">
         <v>369</v>
-      </c>
-      <c r="C143" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
+        <v>370</v>
+      </c>
+      <c r="B144" t="s">
         <v>371</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
         <v>372</v>
-      </c>
-      <c r="C144" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>373</v>
+      </c>
+      <c r="B145" t="s">
         <v>374</v>
       </c>
-      <c r="B145" t="s">
+      <c r="C145" t="s">
         <v>375</v>
-      </c>
-      <c r="C145" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>376</v>
+      </c>
+      <c r="B146" t="s">
         <v>377</v>
       </c>
-      <c r="B146" t="s">
+      <c r="C146" t="s">
         <v>378</v>
-      </c>
-      <c r="C146" t="s">
-        <v>379</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A14:C146 A1:C4 A6:C8 A5:B5" numberStoredAsText="1"/>
+    <ignoredError sqref="A14:C146 A1:C1 A6:C8 A5:B5 A3:C4 A2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance UI components with dark/light theme support and modern design
</commit_message>
<xml_diff>
--- a/frontend/translations/translations.xlsx
+++ b/frontend/translations/translations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D159"/>
+  <dimension ref="A1:D164"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -682,10 +682,10 @@
         <v/>
       </c>
       <c r="C20" t="str">
-        <v>Senior Product Manager</v>
+        <v>Technical Product Manager</v>
       </c>
       <c r="D20" t="str">
-        <v>Quản Lý Sản Phẩm Cao Cấp</v>
+        <v>Quản Lý Sản Phẩm Công Nghệ</v>
       </c>
     </row>
     <row r="21">
@@ -1530,1113 +1530,1183 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>common.published_on</v>
+        <v>common.loading</v>
       </c>
       <c r="B81" t="str">
         <v/>
       </c>
       <c r="C81" t="str">
-        <v>Published on {{date}}</v>
+        <v>Loading...</v>
       </c>
       <c r="D81" t="str">
-        <v>Xuất bản ngày {{date}}</v>
+        <v>Loading...</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>contact.description</v>
+        <v>common.minRead</v>
       </c>
       <c r="B82" t="str">
         <v/>
       </c>
       <c r="C82" t="str">
-        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
+        <v>min read</v>
       </c>
       <c r="D82" t="str">
-        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
+        <v>min read</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>contact.form.email</v>
+        <v>common.published_on</v>
       </c>
       <c r="B83" t="str">
         <v/>
       </c>
       <c r="C83" t="str">
-        <v>Your Email</v>
+        <v>Published on {{date}}</v>
       </c>
       <c r="D83" t="str">
-        <v>Your Email</v>
+        <v>Xuất bản ngày {{date}}</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>contact.form.error</v>
+        <v>common.readMore</v>
       </c>
       <c r="B84" t="str">
         <v/>
       </c>
       <c r="C84" t="str">
-        <v>Error sending message. Please try again.</v>
+        <v>Read more</v>
       </c>
       <c r="D84" t="str">
-        <v>Error sending message. Please try again.</v>
+        <v>Read more</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>contact.form.message</v>
+        <v>contact.description</v>
       </c>
       <c r="B85" t="str">
         <v/>
       </c>
       <c r="C85" t="str">
-        <v>Your Message</v>
+        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
       </c>
       <c r="D85" t="str">
-        <v>Your Message</v>
+        <v>Have a question or want to collaborate? I'd love to hear from you.</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>contact.form.name</v>
+        <v>contact.form.email</v>
       </c>
       <c r="B86" t="str">
         <v/>
       </c>
       <c r="C86" t="str">
-        <v>Your Name</v>
+        <v>Your Email</v>
       </c>
       <c r="D86" t="str">
-        <v>Your Name</v>
+        <v>Your Email</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>contact.form.submit</v>
+        <v>contact.form.error</v>
       </c>
       <c r="B87" t="str">
         <v/>
       </c>
       <c r="C87" t="str">
-        <v>Send Message</v>
+        <v>Error sending message. Please try again.</v>
       </c>
       <c r="D87" t="str">
-        <v>Send Message</v>
+        <v>Error sending message. Please try again.</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>contact.form.success</v>
+        <v>contact.form.message</v>
       </c>
       <c r="B88" t="str">
         <v/>
       </c>
       <c r="C88" t="str">
-        <v>Message sent successfully!</v>
+        <v>Your Message</v>
       </c>
       <c r="D88" t="str">
-        <v>Message sent successfully!</v>
+        <v>Your Message</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>contact.title</v>
+        <v>contact.form.name</v>
       </c>
       <c r="B89" t="str">
         <v/>
       </c>
       <c r="C89" t="str">
-        <v>Get in Touch</v>
+        <v>Your Name</v>
       </c>
       <c r="D89" t="str">
-        <v>Get in Touch</v>
+        <v>Your Name</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>finance.description</v>
+        <v>contact.form.submit</v>
       </c>
       <c r="B90" t="str">
         <v/>
       </c>
       <c r="C90" t="str">
-        <v>Insights and strategies for building financial independence</v>
+        <v>Send Message</v>
       </c>
       <c r="D90" t="str">
-        <v>Những hiểu biết và chiến lược để xây dựng tự do tài chính</v>
+        <v>Send Message</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>finance.sections.budgeting.description</v>
+        <v>contact.form.success</v>
       </c>
       <c r="B91" t="str">
         <v/>
       </c>
       <c r="C91" t="str">
-        <v>Practical tips for effective money management</v>
+        <v>Message sent successfully!</v>
       </c>
       <c r="D91" t="str">
-        <v>Mẹo thực tế để quản lý tiền hiệu quả</v>
+        <v>Message sent successfully!</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>finance.sections.budgeting.title</v>
+        <v>contact.title</v>
       </c>
       <c r="B92" t="str">
         <v/>
       </c>
       <c r="C92" t="str">
-        <v>Smart Budgeting</v>
+        <v>Get in Touch</v>
       </c>
       <c r="D92" t="str">
-        <v>Quản Lý Chi Tiêu</v>
+        <v>Get in Touch</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>finance.sections.investments.description</v>
+        <v>finance.description</v>
       </c>
       <c r="B93" t="str">
         <v/>
       </c>
       <c r="C93" t="str">
-        <v>Long-term approaches to wealth building</v>
+        <v>Insights and strategies for building financial independence</v>
       </c>
       <c r="D93" t="str">
-        <v>Phương pháp xây dựng tài sản dài hạn</v>
+        <v>Những hiểu biết và chiến lược để xây dựng tự do tài chính</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>finance.sections.investments.title</v>
+        <v>finance.sections.budgeting.description</v>
       </c>
       <c r="B94" t="str">
         <v/>
       </c>
       <c r="C94" t="str">
-        <v>Investment Strategies</v>
+        <v>Practical tips for effective money management</v>
       </c>
       <c r="D94" t="str">
-        <v>Chiến Lược Đầu Tư</v>
+        <v>Mẹo thực tế để quản lý tiền hiệu quả</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>finance.sections.planning.description</v>
+        <v>finance.sections.budgeting.title</v>
       </c>
       <c r="B95" t="str">
         <v/>
       </c>
       <c r="C95" t="str">
-        <v>Setting and achieving financial goals</v>
+        <v>Smart Budgeting</v>
       </c>
       <c r="D95" t="str">
-        <v>Thiết lập và đạt được mục tiêu tài chính</v>
+        <v>Quản Lý Chi Tiêu</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>finance.sections.planning.title</v>
+        <v>finance.sections.investments.description</v>
       </c>
       <c r="B96" t="str">
         <v/>
       </c>
       <c r="C96" t="str">
-        <v>Financial Planning</v>
+        <v>Long-term approaches to wealth building</v>
       </c>
       <c r="D96" t="str">
-        <v>Kế Hoạch Tài Chính</v>
+        <v>Phương pháp xây dựng tài sản dài hạn</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>finance.title</v>
+        <v>finance.sections.investments.title</v>
       </c>
       <c r="B97" t="str">
         <v/>
       </c>
       <c r="C97" t="str">
-        <v>Personal Finance</v>
+        <v>Investment Strategies</v>
       </c>
       <c r="D97" t="str">
-        <v>Quản Lý Tài Chính Cá Nhân</v>
+        <v>Chiến Lược Đầu Tư</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>footer.allRightsReserved</v>
+        <v>finance.sections.planning.description</v>
       </c>
       <c r="B98" t="str">
         <v/>
       </c>
       <c r="C98" t="str">
-        <v>All rights reserved.</v>
+        <v>Setting and achieving financial goals</v>
       </c>
       <c r="D98" t="str">
-        <v>All rights reserved.</v>
+        <v>Thiết lập và đạt được mục tiêu tài chính</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>footer.connect</v>
+        <v>finance.sections.planning.title</v>
       </c>
       <c r="B99" t="str">
         <v/>
       </c>
       <c r="C99" t="str">
-        <v>Connect</v>
+        <v>Financial Planning</v>
       </c>
       <c r="D99" t="str">
-        <v>Kết Nối</v>
+        <v>Kế Hoạch Tài Chính</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>footer.privacyPolicy</v>
+        <v>finance.title</v>
       </c>
       <c r="B100" t="str">
         <v/>
       </c>
       <c r="C100" t="str">
-        <v>Privacy Policy</v>
+        <v>Personal Finance</v>
       </c>
       <c r="D100" t="str">
-        <v>Privacy Policy</v>
+        <v>Quản Lý Tài Chính Cá Nhân</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>footer.quickLinks</v>
+        <v>footer.allRightsReserved</v>
       </c>
       <c r="B101" t="str">
         <v/>
       </c>
       <c r="C101" t="str">
-        <v>Quick access</v>
+        <v>All rights reserved.</v>
       </c>
       <c r="D101" t="str">
-        <v>Liên Kết Nhanh</v>
+        <v>All rights reserved.</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>footer.stayUpdated</v>
+        <v>footer.connect</v>
       </c>
       <c r="B102" t="str">
         <v/>
       </c>
       <c r="C102" t="str">
-        <v>Stay updated with the latest insights</v>
+        <v>Connect</v>
       </c>
       <c r="D102" t="str">
-        <v>Stay updated with the latest insights</v>
+        <v>Kết Nối</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>footer.termsOfService</v>
+        <v>footer.privacyPolicy</v>
       </c>
       <c r="B103" t="str">
         <v/>
       </c>
       <c r="C103" t="str">
-        <v>Terms of Service</v>
+        <v>Privacy Policy</v>
       </c>
       <c r="D103" t="str">
-        <v>Terms of Service</v>
+        <v>Privacy Policy</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>hero.cta.primary</v>
+        <v>footer.quickLinks</v>
       </c>
       <c r="B104" t="str">
         <v/>
       </c>
       <c r="C104" t="str">
-        <v>Explore Resources</v>
+        <v>Quick access</v>
       </c>
       <c r="D104" t="str">
-        <v>Khám Phá Tài Nguyên</v>
+        <v>Liên Kết Nhanh</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>hero.cta.secondary</v>
+        <v>footer.stayUpdated</v>
       </c>
       <c r="B105" t="str">
         <v/>
       </c>
       <c r="C105" t="str">
-        <v>View Blog</v>
+        <v>Stay updated with the latest insights</v>
       </c>
       <c r="D105" t="str">
-        <v>Xem Blog</v>
+        <v>Stay updated with the latest insights</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>hero.description</v>
+        <v>footer.termsOfService</v>
       </c>
       <c r="B106" t="str">
         <v/>
       </c>
       <c r="C106" t="str">
-        <v>Exploring the intersection of technology and social impact through thoughtful analysis and practical insights</v>
+        <v>Terms of Service</v>
       </c>
       <c r="D106" t="str">
-        <v>Khám phá sự giao thoa giữa công nghệ và tác động xã hội thông qua phân tích sâu sắc và những hiểu biết thực tế</v>
+        <v>Terms of Service</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>hero.subtitle</v>
+        <v>hero.cta.primary</v>
       </c>
       <c r="B107" t="str">
         <v/>
       </c>
       <c r="C107" t="str">
-        <v>Discover insights on technology, personal growth, and making a positive impact</v>
+        <v>Explore Resources</v>
       </c>
       <c r="D107" t="str">
-        <v>Khám phá những hiểu biết về công nghệ, phát triển bản thân và tạo tác động tích cực</v>
+        <v>Khám Phá Tài Nguyên</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>hero.title</v>
+        <v>hero.cta.secondary</v>
       </c>
       <c r="B108" t="str">
         <v/>
       </c>
       <c r="C108" t="str">
-        <v>Welcome to My Knowledge Hub</v>
+        <v>View Blog</v>
       </c>
       <c r="D108" t="str">
-        <v>Chào Mừng Đến Với Kho Kiến Thức</v>
+        <v>Xem Blog</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>impact.description</v>
+        <v>hero.description</v>
       </c>
       <c r="B109" t="str">
         <v/>
       </c>
       <c r="C109" t="str">
-        <v>Making a positive difference in the world</v>
+        <v>Exploring the intersection of technology and social impact through thoughtful analysis and practical insights</v>
       </c>
       <c r="D109" t="str">
-        <v>Tạo ra những thay đổi tích cực cho thế giới</v>
+        <v>Khám phá sự giao thoa giữa công nghệ và tác động xã hội thông qua phân tích sâu sắc và những hiểu biết thực tế</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>impact.no_projects</v>
+        <v>hero.subtitle</v>
       </c>
       <c r="B110" t="str">
         <v/>
       </c>
       <c r="C110" t="str">
-        <v>Nothing show here</v>
+        <v>Discover insights on technology, personal growth, and making a positive impact</v>
       </c>
       <c r="D110" t="str">
-        <v>Chưa có dự án nào</v>
+        <v>Khám phá những hiểu biết về công nghệ, phát triển bản thân và tạo tác động tích cực</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>impact.sections.collaboration.description</v>
+        <v>hero.title</v>
       </c>
       <c r="B111" t="str">
         <v/>
       </c>
       <c r="C111" t="str">
-        <v>Ways to contribute and collaborate</v>
+        <v>Welcome to My Knowledge Hub</v>
       </c>
       <c r="D111" t="str">
-        <v>Cách đóng góp và hợp tác</v>
+        <v>Chào Mừng Đến Với Kho Kiến Thức</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>impact.sections.collaboration.title</v>
+        <v>impact.description</v>
       </c>
       <c r="B112" t="str">
         <v/>
       </c>
       <c r="C112" t="str">
-        <v>Get Involved</v>
+        <v>Making a positive difference in the world</v>
       </c>
       <c r="D112" t="str">
-        <v>Tham Gia</v>
+        <v>Tạo ra những thay đổi tích cực cho thế giới</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>impact.sections.metrics.description</v>
+        <v>impact.no_projects</v>
       </c>
       <c r="B113" t="str">
         <v/>
       </c>
       <c r="C113" t="str">
-        <v>Measuring and tracking social impact</v>
+        <v>Nothing show here</v>
       </c>
       <c r="D113" t="str">
-        <v>Đo lường và theo dõi tác động xã hội</v>
+        <v>Chưa có dự án nào</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>impact.sections.metrics.title</v>
+        <v>impact.sections.collaboration.description</v>
       </c>
       <c r="B114" t="str">
         <v/>
       </c>
       <c r="C114" t="str">
-        <v>Impact Metrics</v>
+        <v>Ways to contribute and collaborate</v>
       </c>
       <c r="D114" t="str">
-        <v>Đo Lường Tác Động</v>
+        <v>Cách đóng góp và hợp tác</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>impact.sections.projects.description</v>
+        <v>impact.sections.collaboration.title</v>
       </c>
       <c r="B115" t="str">
         <v/>
       </c>
       <c r="C115" t="str">
-        <v>Current initiatives and their outcomes</v>
+        <v>Get Involved</v>
       </c>
       <c r="D115" t="str">
-        <v>Các sáng kiến hiện tại và kết quả</v>
+        <v>Tham Gia</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>impact.sections.projects.title</v>
+        <v>impact.sections.metrics.description</v>
       </c>
       <c r="B116" t="str">
         <v/>
       </c>
       <c r="C116" t="str">
-        <v>Impact Projects</v>
+        <v>Measuring and tracking social impact</v>
       </c>
       <c r="D116" t="str">
-        <v>Dự Án Tác Động</v>
+        <v>Đo lường và theo dõi tác động xã hội</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>impact.title</v>
+        <v>impact.sections.metrics.title</v>
       </c>
       <c r="B117" t="str">
         <v/>
       </c>
       <c r="C117" t="str">
-        <v>Social Impact</v>
+        <v>Impact Metrics</v>
       </c>
       <c r="D117" t="str">
-        <v>Tác Động Xã Hội</v>
+        <v>Đo Lường Tác Động</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>library.book_not_found</v>
+        <v>impact.sections.projects.description</v>
       </c>
       <c r="B118" t="str">
         <v/>
       </c>
       <c r="C118" t="str">
-        <v>Book not found</v>
+        <v>Current initiatives and their outcomes</v>
       </c>
       <c r="D118" t="str">
-        <v>Không tìm thấy sách</v>
+        <v>Các sáng kiến hiện tại và kết quả</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>library.book_not_found_description</v>
+        <v>impact.sections.projects.title</v>
       </c>
       <c r="B119" t="str">
         <v/>
       </c>
       <c r="C119" t="str">
-        <v>Sorry, we couldn't find the book you're looking for.</v>
+        <v>Impact Projects</v>
       </c>
       <c r="D119" t="str">
-        <v>Xin lỗi, chúng tôi không thể tìm thấy cuốn sách bạn đang tìm kiếm.</v>
+        <v>Dự Án Tác Động</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>library.by</v>
+        <v>impact.title</v>
       </c>
       <c r="B120" t="str">
         <v/>
       </c>
       <c r="C120" t="str">
-        <v>by</v>
+        <v>Social Impact</v>
       </c>
       <c r="D120" t="str">
-        <v>bởi</v>
+        <v>Tác Động Xã Hội</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>library.chapter</v>
+        <v>library.book_not_found</v>
       </c>
       <c r="B121" t="str">
         <v/>
       </c>
       <c r="C121" t="str">
-        <v>Chapter {{number}}</v>
+        <v>Book not found</v>
       </c>
       <c r="D121" t="str">
-        <v>Chương {{number}}</v>
+        <v>Không tìm thấy sách</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>library.key_takeaways</v>
+        <v>library.book_not_found_description</v>
       </c>
       <c r="B122" t="str">
         <v/>
       </c>
       <c r="C122" t="str">
-        <v>Key Takeaways</v>
+        <v>Sorry, we couldn't find the book you're looking for.</v>
       </c>
       <c r="D122" t="str">
-        <v>Điểm Chính</v>
+        <v>Xin lỗi, chúng tôi không thể tìm thấy cuốn sách bạn đang tìm kiếm.</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>library.last_updated</v>
+        <v>library.by</v>
       </c>
       <c r="B123" t="str">
         <v/>
       </c>
       <c r="C123" t="str">
-        <v>Last updated {{date}}</v>
+        <v>by</v>
       </c>
       <c r="D123" t="str">
-        <v>Cập nhật lần cuối {{date}}</v>
+        <v>bởi</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>library.latest_read</v>
+        <v>library.chapter</v>
       </c>
       <c r="B124" t="str">
         <v/>
       </c>
       <c r="C124" t="str">
-        <v>Latest Read</v>
+        <v>Chapter {{number}}</v>
       </c>
       <c r="D124" t="str">
-        <v>Sách Mới Nhất</v>
+        <v>Chương {{number}}</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>library.next_chapter</v>
+        <v>library.key_takeaways</v>
       </c>
       <c r="B125" t="str">
         <v/>
       </c>
       <c r="C125" t="str">
-        <v>Next Chapter</v>
+        <v>Key Takeaways</v>
       </c>
       <c r="D125" t="str">
-        <v>Chương Tiếp Theo</v>
+        <v>Điểm Chính</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>library.previous_chapter</v>
+        <v>library.last_updated</v>
       </c>
       <c r="B126" t="str">
         <v/>
       </c>
       <c r="C126" t="str">
-        <v>Previous Chapter</v>
+        <v>Last updated {{date}}</v>
       </c>
       <c r="D126" t="str">
-        <v>Chương Trước</v>
+        <v>Cập nhật lần cuối {{date}}</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>library.read_notes</v>
+        <v>library.latest_read</v>
       </c>
       <c r="B127" t="str">
         <v/>
       </c>
       <c r="C127" t="str">
-        <v>Read My Notes</v>
+        <v>Latest Read</v>
       </c>
       <c r="D127" t="str">
-        <v>Xem Ghi Chú</v>
+        <v>Sách Mới Nhất</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>library.reading_time</v>
+        <v>library.next_chapter</v>
       </c>
       <c r="B128" t="str">
         <v/>
       </c>
       <c r="C128" t="str">
-        <v>{{minutes}} min read</v>
+        <v>Next Chapter</v>
       </c>
       <c r="D128" t="str">
-        <v>{{minutes}} phút đọc</v>
+        <v>Chương Tiếp Theo</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>library.section_description</v>
+        <v>library.previous_chapter</v>
       </c>
       <c r="B129" t="str">
         <v/>
       </c>
       <c r="C129" t="str">
-        <v>Here are the books I've read and my key takeaways from each one. I hope these notes inspire you to pick up one of these books.</v>
+        <v>Previous Chapter</v>
       </c>
       <c r="D129" t="str">
-        <v>Đây là những cuốn sách tôi đã đọc và những điểm chính tôi rút ra từ mỗi cuốn. Hy vọng những ghi chú này sẽ truyền cảm hứng cho bạn đọc những cuốn sách này.</v>
+        <v>Chương Trước</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>library.section_title</v>
+        <v>library.read_notes</v>
       </c>
       <c r="B130" t="str">
         <v/>
       </c>
       <c r="C130" t="str">
-        <v>My Book Notes</v>
+        <v>Read My Notes</v>
       </c>
       <c r="D130" t="str">
-        <v>Ghi Chú Sách</v>
+        <v>Xem Ghi Chú</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>library.table_of_contents</v>
+        <v>library.reading_time</v>
       </c>
       <c r="B131" t="str">
         <v/>
       </c>
       <c r="C131" t="str">
-        <v>Table of Contents</v>
+        <v>{{minutes}} min read</v>
       </c>
       <c r="D131" t="str">
-        <v>Mục Lục</v>
+        <v>{{minutes}} phút đọc</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>meta.home.description</v>
+        <v>library.section_description</v>
       </c>
       <c r="B132" t="str">
         <v/>
       </c>
       <c r="C132" t="str">
-        <v>My personal website has knowledge about technology, personal growth, and making impacts on society.</v>
+        <v>Here are the books I've read and my key takeaways from each one. I hope these notes inspire you to pick up one of these books.</v>
       </c>
       <c r="D132" t="str">
-        <v>Trang web cá nhân với những hiểu biết về công nghệ, phát triển bản thân và tạo tác động tích cực</v>
+        <v>Đây là những cuốn sách tôi đã đọc và những điểm chính tôi rút ra từ mỗi cuốn. Hy vọng những ghi chú này sẽ truyền cảm hứng cho bạn đọc những cuốn sách này.</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>meta.home.title</v>
+        <v>library.section_title</v>
       </c>
       <c r="B133" t="str">
         <v/>
       </c>
       <c r="C133" t="str">
-        <v>Home | KienNotes.AI</v>
+        <v>My Book Notes</v>
       </c>
       <c r="D133" t="str">
-        <v>Trang Chủ | KienNotes.AI</v>
+        <v>Ghi Chú Sách</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>nav.about</v>
+        <v>library.table_of_contents</v>
       </c>
       <c r="B134" t="str">
         <v/>
       </c>
       <c r="C134" t="str">
-        <v>About</v>
+        <v>Table of Contents</v>
       </c>
       <c r="D134" t="str">
-        <v>Giới Thiệu</v>
+        <v>Mục Lục</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>nav.blog</v>
+        <v>library.title</v>
       </c>
       <c r="B135" t="str">
         <v/>
       </c>
       <c r="C135" t="str">
-        <v>Blog</v>
+        <v>Resource Library</v>
       </c>
       <c r="D135" t="str">
-        <v>Blog</v>
+        <v>Resource Library</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>nav.finance</v>
+        <v>meta.home.description</v>
       </c>
       <c r="B136" t="str">
         <v/>
       </c>
       <c r="C136" t="str">
-        <v>Finance</v>
+        <v>My personal website has knowledge about technology, personal growth, and making impacts on society.</v>
       </c>
       <c r="D136" t="str">
-        <v>Tài Chính Cá Nhân</v>
+        <v>Trang web cá nhân với những hiểu biết về công nghệ, phát triển bản thân và tạo tác động tích cực</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>nav.home</v>
+        <v>meta.home.title</v>
       </c>
       <c r="B137" t="str">
         <v/>
       </c>
       <c r="C137" t="str">
-        <v>Home</v>
+        <v>Home | KienNotes.AI</v>
       </c>
       <c r="D137" t="str">
-        <v>Trang Chủ</v>
+        <v>Trang Chủ | KienNotes.AI</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>nav.impact</v>
+        <v>nav.about</v>
       </c>
       <c r="B138" t="str">
         <v/>
       </c>
       <c r="C138" t="str">
-        <v>Impact</v>
+        <v>About</v>
       </c>
       <c r="D138" t="str">
-        <v>Tác Động Xã Hội</v>
+        <v>Giới Thiệu</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>nav.library</v>
+        <v>nav.blog</v>
       </c>
       <c r="B139" t="str">
         <v/>
       </c>
       <c r="C139" t="str">
-        <v>Library</v>
+        <v>Blog</v>
       </c>
       <c r="D139" t="str">
-        <v>Thư viện</v>
+        <v>Blog</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>nav.login</v>
+        <v>nav.finance</v>
       </c>
       <c r="B140" t="str">
         <v/>
       </c>
       <c r="C140" t="str">
-        <v>Login</v>
+        <v>Finance</v>
       </c>
       <c r="D140" t="str">
-        <v>Đăng nhập</v>
+        <v>Tài Chính Cá Nhân</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>nav.logout</v>
+        <v>nav.home</v>
       </c>
       <c r="B141" t="str">
         <v/>
       </c>
       <c r="C141" t="str">
-        <v>Log Out</v>
+        <v>Home</v>
       </c>
       <c r="D141" t="str">
-        <v>Đăng xuất</v>
+        <v>Trang Chủ</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>nav.profile</v>
+        <v>nav.impact</v>
       </c>
       <c r="B142" t="str">
         <v/>
       </c>
       <c r="C142" t="str">
-        <v>Profile</v>
+        <v>Impact</v>
       </c>
       <c r="D142" t="str">
-        <v>Tài khoản của bạn</v>
+        <v>Tác Động Xã Hội</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>nav.signup</v>
+        <v>nav.library</v>
       </c>
       <c r="B143" t="str">
         <v/>
       </c>
       <c r="C143" t="str">
-        <v>Sign up</v>
+        <v>Library</v>
       </c>
       <c r="D143" t="str">
-        <v>Đăng ký</v>
+        <v>Thư viện</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>newsletter.button</v>
+        <v>nav.login</v>
       </c>
       <c r="B144" t="str">
         <v/>
       </c>
       <c r="C144" t="str">
-        <v>Subscribe</v>
+        <v>Login</v>
       </c>
       <c r="D144" t="str">
-        <v>Đăng Ký</v>
+        <v>Đăng nhập</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>newsletter.description</v>
+        <v>nav.logout</v>
       </c>
       <c r="B145" t="str">
         <v/>
       </c>
       <c r="C145" t="str">
-        <v>Get the latest insights delivered to your inbox</v>
+        <v>Log Out</v>
       </c>
       <c r="D145" t="str">
-        <v>Nhận những thông tin mới nhất qua email</v>
+        <v>Đăng xuất</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>newsletter.error</v>
+        <v>nav.profile</v>
       </c>
       <c r="B146" t="str">
         <v/>
       </c>
       <c r="C146" t="str">
-        <v>Something went wrong. Please try again.</v>
+        <v>Profile</v>
       </c>
       <c r="D146" t="str">
-        <v>Đã xảy ra lỗi. Vui lòng thử lại.</v>
+        <v>Tài khoản của bạn</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>newsletter.placeholder</v>
+        <v>nav.signup</v>
       </c>
       <c r="B147" t="str">
         <v/>
       </c>
       <c r="C147" t="str">
-        <v>Enter your email</v>
+        <v>Sign up</v>
       </c>
       <c r="D147" t="str">
-        <v>Nhập email của bạn</v>
+        <v>Đăng ký</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>newsletter.success</v>
+        <v>newsletter.button</v>
       </c>
       <c r="B148" t="str">
         <v/>
       </c>
       <c r="C148" t="str">
-        <v>Thank you for subscribing!</v>
+        <v>Subscribe</v>
       </c>
       <c r="D148" t="str">
-        <v>Cảm ơn bạn đã đăng ký!</v>
+        <v>Đăng Ký</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>newsletter.title</v>
+        <v>newsletter.description</v>
       </c>
       <c r="B149" t="str">
         <v/>
       </c>
       <c r="C149" t="str">
-        <v>Subscribe to Newsletter</v>
+        <v>Get the latest insights delivered to your inbox</v>
       </c>
       <c r="D149" t="str">
-        <v>Đăng Ký Nhận Bản Tin</v>
+        <v>Nhận những thông tin mới nhất qua email</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>resources.description</v>
+        <v>newsletter.error</v>
       </c>
       <c r="B150" t="str">
         <v/>
       </c>
       <c r="C150" t="str">
-        <v>A collection of tools, guides, and resources to help you on your journey</v>
+        <v>Something went wrong. Please try again.</v>
       </c>
       <c r="D150" t="str">
-        <v>Bộ sưu tập công cụ, hướng dẫn và tài nguyên để hỗ trợ bạn trên hành trình của mình</v>
+        <v>Đã xảy ra lỗi. Vui lòng thử lại.</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>resources.guides</v>
+        <v>newsletter.invalidEmail</v>
       </c>
       <c r="B151" t="str">
         <v/>
       </c>
       <c r="C151" t="str">
-        <v>Guides</v>
+        <v>Please enter a valid email address</v>
       </c>
       <c r="D151" t="str">
-        <v>Hướng Dẫn</v>
+        <v>Please enter a valid email address</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>resources.title</v>
+        <v>newsletter.placeholder</v>
       </c>
       <c r="B152" t="str">
         <v/>
       </c>
       <c r="C152" t="str">
-        <v>Resources</v>
+        <v>Enter your email</v>
       </c>
       <c r="D152" t="str">
-        <v>Tài Nguyên</v>
+        <v>Nhập email của bạn</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>resources.tools</v>
+        <v>newsletter.success</v>
       </c>
       <c r="B153" t="str">
         <v/>
       </c>
       <c r="C153" t="str">
-        <v>Tools</v>
+        <v>Thank you for subscribing!</v>
       </c>
       <c r="D153" t="str">
-        <v>Công Cụ</v>
+        <v>Cảm ơn bạn đã đăng ký!</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>site.author</v>
+        <v>newsletter.title</v>
       </c>
       <c r="B154" t="str">
         <v/>
       </c>
       <c r="C154" t="str">
-        <v>John Anderson</v>
+        <v>Subscribe to Newsletter</v>
       </c>
       <c r="D154" t="str">
-        <v>John Anderson</v>
+        <v>Đăng Ký Nhận Bản Tin</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>site.description</v>
+        <v>resources.description</v>
       </c>
       <c r="B155" t="str">
         <v/>
       </c>
       <c r="C155" t="str">
-        <v>Discover insights on technology, personal growth, and making a positive impact</v>
+        <v>A collection of tools, guides, and resources to help you on your journey</v>
       </c>
       <c r="D155" t="str">
-        <v>Khám phá những hiểu biết về công nghệ, phát triển bản thân và tạo tác động tích cực</v>
+        <v>Bộ sưu tập công cụ, hướng dẫn và tài nguyên để hỗ trợ bạn trên hành trình của mình</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>site.tagline</v>
+        <v>resources.guides</v>
       </c>
       <c r="B156" t="str">
         <v/>
       </c>
       <c r="C156" t="str">
-        <v>Building innovative solutions for a better tomorrow</v>
+        <v>Guides</v>
       </c>
       <c r="D156" t="str">
-        <v>Building innovative solutions for a better tomorrow</v>
+        <v>Hướng Dẫn</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>site.title</v>
+        <v>resources.title</v>
       </c>
       <c r="B157" t="str">
         <v/>
       </c>
       <c r="C157" t="str">
-        <v>KienNotes.AI</v>
+        <v>Resources</v>
       </c>
       <c r="D157" t="str">
-        <v>KienNotes.AI</v>
+        <v>Tài Nguyên</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>theme.dark</v>
+        <v>resources.tools</v>
       </c>
       <c r="B158" t="str">
         <v/>
       </c>
       <c r="C158" t="str">
-        <v>Dark mode</v>
+        <v>Tools</v>
       </c>
       <c r="D158" t="str">
-        <v>Chế độ tối</v>
+        <v>Công Cụ</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
+        <v>site.author</v>
+      </c>
+      <c r="B159" t="str">
+        <v/>
+      </c>
+      <c r="C159" t="str">
+        <v>Kien (Jonathan) Vu Viet</v>
+      </c>
+      <c r="D159" t="str">
+        <v>Kiên (Jonathan) Vũ Viết</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>site.description</v>
+      </c>
+      <c r="B160" t="str">
+        <v/>
+      </c>
+      <c r="C160" t="str">
+        <v>Discover insights on technology, personal growth, and making a positive impact</v>
+      </c>
+      <c r="D160" t="str">
+        <v>Khám phá những hiểu biết về công nghệ, phát triển bản thân và tạo tác động tích cực</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>site.tagline</v>
+      </c>
+      <c r="B161" t="str">
+        <v/>
+      </c>
+      <c r="C161" t="str">
+        <v>Building innovative solutions for a better tomorrow</v>
+      </c>
+      <c r="D161" t="str">
+        <v>Building innovative solutions for a better tomorrow</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>site.title</v>
+      </c>
+      <c r="B162" t="str">
+        <v/>
+      </c>
+      <c r="C162" t="str">
+        <v>KienNotes.AI</v>
+      </c>
+      <c r="D162" t="str">
+        <v>KienNotes.AI</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v>theme.dark</v>
+      </c>
+      <c r="B163" t="str">
+        <v/>
+      </c>
+      <c r="C163" t="str">
+        <v>Dark mode</v>
+      </c>
+      <c r="D163" t="str">
+        <v>Chế độ tối</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
         <v>theme.light</v>
       </c>
-      <c r="B159" t="str">
-        <v/>
-      </c>
-      <c r="C159" t="str">
+      <c r="B164" t="str">
+        <v/>
+      </c>
+      <c r="C164" t="str">
         <v>Light mode</v>
       </c>
-      <c r="D159" t="str">
+      <c r="D164" t="str">
         <v>Chế độ sáng</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D159"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D164"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>